<commit_message>
Fixing sampling type bug
</commit_message>
<xml_diff>
--- a/raw/project_UVP_standardizer.xlsx
+++ b/raw/project_UVP_standardizer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="313">
   <si>
     <t>Project_ID</t>
   </si>
@@ -429,6 +429,186 @@
   </si>
   <si>
     <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_110_20221007_1442_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_214_20220929_1318_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_507_20220929_1325_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_545_20220929_1328_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_548_20221008_1224_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_556_20220929_1817_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_558_20220929_1821_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_559_20220929_1823_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_560_20220609_1315_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_563_20220929_1828_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_579_20220609_1319_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_584_20220829_1544_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_585_20221008_1235_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_586_20220929_1844_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_587_20220929_1845_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_588_20220929_1845_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_589_20220929_1846_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_590_20220929_1849_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_593_20220829_1547_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_594_20220929_1851_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_595_20220929_1851_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_602_20221008_1237_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_603_20220930_0408_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_610_20220930_0415_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_620_20221007_1444_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_621_20220930_0515_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_622_20220829_1554_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_651_20220930_0520_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_855_20221007_1452_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_881_20221007_1456_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_1343_20221008_1046_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_2465_20221007_1507_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_2483_20221007_1511_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_2806_20221007_1532_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_2807_20221007_1533_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_2808_20221007_1538_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_3117_20221007_1543_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_3403_20221008_1115_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_5197_20221008_1127_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_5208_20221008_1134_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_5680_20221007_1544_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_5690_20221007_1548_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_5693_20220610_0940_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_6047_20221007_1614_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_6702_20221008_1159_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_6703_20221008_1201_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_6704_20221008_1208_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_3_20221012_0944_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_4_20221012_0946_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_28_20221012_0954_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_36_20221012_0958_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_37_20221012_1001_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_38_20221012_1005_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_39_20221012_1007_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_578_20221012_1021_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_3278_20221012_1056_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_3327_20221012_1057_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_3887_20221012_1059_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_3943_20221012_1059_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_4591_20221012_1103_flags.tsv</t>
+  </si>
+  <si>
+    <t>~/GIT/PSSdb/raw/flags/UVP/ecotaxa_export_5254_20221012_1136_flags.tsv</t>
   </si>
   <si>
     <t>uvp5_sn003_sargasso_a,uvp5_sn003_sargasso_b</t>
@@ -1385,19 +1565,19 @@
         <v>136</v>
       </c>
       <c r="AM2" t="s">
-        <v>138</v>
+        <v>198</v>
       </c>
       <c r="AN2" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO2" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP2" t="s">
         <v>129</v>
       </c>
       <c r="AS2" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -1498,19 +1678,19 @@
         <v>137</v>
       </c>
       <c r="AM3" t="s">
-        <v>139</v>
+        <v>199</v>
       </c>
       <c r="AN3" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO3" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP3" t="s">
         <v>129</v>
       </c>
       <c r="AS3" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:45">
@@ -1607,20 +1787,23 @@
       <c r="AJ4" t="s">
         <v>135</v>
       </c>
+      <c r="AK4" t="s">
+        <v>138</v>
+      </c>
       <c r="AM4" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="AN4" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO4" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP4" t="s">
         <v>129</v>
       </c>
       <c r="AS4" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -1717,20 +1900,23 @@
       <c r="AJ5" t="s">
         <v>135</v>
       </c>
+      <c r="AK5" t="s">
+        <v>139</v>
+      </c>
       <c r="AM5" t="s">
-        <v>141</v>
+        <v>201</v>
       </c>
       <c r="AN5" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO5" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP5" t="s">
         <v>129</v>
       </c>
       <c r="AS5" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -1827,20 +2013,23 @@
       <c r="AJ6" t="s">
         <v>135</v>
       </c>
+      <c r="AK6" t="s">
+        <v>140</v>
+      </c>
       <c r="AM6" t="s">
-        <v>142</v>
+        <v>202</v>
       </c>
       <c r="AN6" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO6" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP6" t="s">
         <v>129</v>
       </c>
       <c r="AS6" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -1937,20 +2126,23 @@
       <c r="AJ7" t="s">
         <v>135</v>
       </c>
+      <c r="AK7" t="s">
+        <v>141</v>
+      </c>
       <c r="AM7" t="s">
-        <v>143</v>
+        <v>203</v>
       </c>
       <c r="AN7" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO7" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP7" t="s">
         <v>129</v>
       </c>
       <c r="AS7" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -2047,14 +2239,17 @@
       <c r="AJ8" t="s">
         <v>135</v>
       </c>
+      <c r="AK8" t="s">
+        <v>142</v>
+      </c>
       <c r="AM8" t="s">
-        <v>144</v>
+        <v>204</v>
       </c>
       <c r="AN8" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS8" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -2151,14 +2346,17 @@
       <c r="AJ9" t="s">
         <v>135</v>
       </c>
+      <c r="AK9" t="s">
+        <v>143</v>
+      </c>
       <c r="AM9" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
       <c r="AN9" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS9" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -2255,20 +2453,23 @@
       <c r="AJ10" t="s">
         <v>135</v>
       </c>
+      <c r="AK10" t="s">
+        <v>144</v>
+      </c>
       <c r="AM10" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="AN10" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO10" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP10" t="s">
         <v>129</v>
       </c>
       <c r="AS10" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:45">
@@ -2365,20 +2566,23 @@
       <c r="AJ11" t="s">
         <v>135</v>
       </c>
+      <c r="AK11" t="s">
+        <v>145</v>
+      </c>
       <c r="AM11" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="AN11" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO11" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP11" t="s">
         <v>129</v>
       </c>
       <c r="AS11" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:45">
@@ -2475,20 +2679,23 @@
       <c r="AJ12" t="s">
         <v>135</v>
       </c>
+      <c r="AK12" t="s">
+        <v>146</v>
+      </c>
       <c r="AM12" t="s">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="AN12" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO12" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP12" t="s">
         <v>129</v>
       </c>
       <c r="AS12" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:45">
@@ -2585,20 +2792,23 @@
       <c r="AJ13" t="s">
         <v>135</v>
       </c>
+      <c r="AK13" t="s">
+        <v>147</v>
+      </c>
       <c r="AM13" t="s">
-        <v>149</v>
+        <v>209</v>
       </c>
       <c r="AN13" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO13" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP13" t="s">
         <v>129</v>
       </c>
       <c r="AS13" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:45">
@@ -2695,20 +2905,23 @@
       <c r="AJ14" t="s">
         <v>135</v>
       </c>
+      <c r="AK14" t="s">
+        <v>148</v>
+      </c>
       <c r="AM14" t="s">
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="AN14" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO14" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP14" t="s">
         <v>129</v>
       </c>
       <c r="AS14" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:45">
@@ -2805,14 +3018,17 @@
       <c r="AJ15" t="s">
         <v>135</v>
       </c>
+      <c r="AK15" t="s">
+        <v>149</v>
+      </c>
       <c r="AM15" t="s">
-        <v>151</v>
+        <v>211</v>
       </c>
       <c r="AN15" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS15" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:45">
@@ -2909,20 +3125,23 @@
       <c r="AJ16" t="s">
         <v>135</v>
       </c>
+      <c r="AK16" t="s">
+        <v>150</v>
+      </c>
       <c r="AM16" t="s">
-        <v>152</v>
+        <v>212</v>
       </c>
       <c r="AN16" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO16" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP16" t="s">
         <v>129</v>
       </c>
       <c r="AS16" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:45">
@@ -3019,14 +3238,17 @@
       <c r="AJ17" t="s">
         <v>135</v>
       </c>
+      <c r="AK17" t="s">
+        <v>151</v>
+      </c>
       <c r="AM17" t="s">
-        <v>153</v>
+        <v>213</v>
       </c>
       <c r="AN17" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS17" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:45">
@@ -3123,20 +3345,23 @@
       <c r="AJ18" t="s">
         <v>135</v>
       </c>
+      <c r="AK18" t="s">
+        <v>152</v>
+      </c>
       <c r="AM18" t="s">
-        <v>154</v>
+        <v>214</v>
       </c>
       <c r="AN18" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO18" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP18" t="s">
         <v>129</v>
       </c>
       <c r="AS18" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:45">
@@ -3233,20 +3458,23 @@
       <c r="AJ19" t="s">
         <v>135</v>
       </c>
+      <c r="AK19" t="s">
+        <v>153</v>
+      </c>
       <c r="AM19" t="s">
-        <v>155</v>
+        <v>215</v>
       </c>
       <c r="AN19" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO19" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP19" t="s">
         <v>129</v>
       </c>
       <c r="AS19" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:45">
@@ -3343,20 +3571,23 @@
       <c r="AJ20" t="s">
         <v>135</v>
       </c>
+      <c r="AK20" t="s">
+        <v>154</v>
+      </c>
       <c r="AM20" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="AN20" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO20" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP20" t="s">
         <v>129</v>
       </c>
       <c r="AS20" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:45">
@@ -3453,14 +3684,17 @@
       <c r="AJ21" t="s">
         <v>135</v>
       </c>
+      <c r="AK21" t="s">
+        <v>155</v>
+      </c>
       <c r="AM21" t="s">
-        <v>157</v>
+        <v>217</v>
       </c>
       <c r="AN21" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS21" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:45">
@@ -3557,20 +3791,23 @@
       <c r="AJ22" t="s">
         <v>135</v>
       </c>
+      <c r="AK22" t="s">
+        <v>156</v>
+      </c>
       <c r="AM22" t="s">
-        <v>158</v>
+        <v>218</v>
       </c>
       <c r="AN22" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO22" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP22" t="s">
         <v>129</v>
       </c>
       <c r="AS22" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:45">
@@ -3667,20 +3904,23 @@
       <c r="AJ23" t="s">
         <v>135</v>
       </c>
+      <c r="AK23" t="s">
+        <v>157</v>
+      </c>
       <c r="AM23" t="s">
-        <v>159</v>
+        <v>219</v>
       </c>
       <c r="AN23" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO23" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP23" t="s">
         <v>129</v>
       </c>
       <c r="AS23" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:45">
@@ -3777,14 +4017,17 @@
       <c r="AJ24" t="s">
         <v>135</v>
       </c>
+      <c r="AK24" t="s">
+        <v>158</v>
+      </c>
       <c r="AM24" t="s">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="AN24" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS24" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:45">
@@ -3881,14 +4124,17 @@
       <c r="AJ25" t="s">
         <v>135</v>
       </c>
+      <c r="AK25" t="s">
+        <v>159</v>
+      </c>
       <c r="AM25" t="s">
-        <v>161</v>
+        <v>221</v>
       </c>
       <c r="AN25" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS25" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:45">
@@ -3985,14 +4231,17 @@
       <c r="AJ26" t="s">
         <v>135</v>
       </c>
+      <c r="AK26" t="s">
+        <v>160</v>
+      </c>
       <c r="AM26" t="s">
-        <v>162</v>
+        <v>222</v>
       </c>
       <c r="AN26" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS26" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:45">
@@ -4089,20 +4338,23 @@
       <c r="AJ27" t="s">
         <v>135</v>
       </c>
+      <c r="AK27" t="s">
+        <v>161</v>
+      </c>
       <c r="AM27" t="s">
-        <v>163</v>
+        <v>223</v>
       </c>
       <c r="AN27" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO27" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP27" t="s">
         <v>129</v>
       </c>
       <c r="AS27" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:45">
@@ -4199,20 +4451,23 @@
       <c r="AJ28" t="s">
         <v>135</v>
       </c>
+      <c r="AK28" t="s">
+        <v>162</v>
+      </c>
       <c r="AM28" t="s">
-        <v>164</v>
+        <v>224</v>
       </c>
       <c r="AN28" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO28" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP28" t="s">
         <v>129</v>
       </c>
       <c r="AS28" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:45">
@@ -4309,14 +4564,17 @@
       <c r="AJ29" t="s">
         <v>135</v>
       </c>
+      <c r="AK29" t="s">
+        <v>163</v>
+      </c>
       <c r="AM29" t="s">
-        <v>165</v>
+        <v>225</v>
       </c>
       <c r="AN29" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS29" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:45">
@@ -4413,20 +4671,23 @@
       <c r="AJ30" t="s">
         <v>135</v>
       </c>
+      <c r="AK30" t="s">
+        <v>164</v>
+      </c>
       <c r="AM30" t="s">
-        <v>166</v>
+        <v>226</v>
       </c>
       <c r="AN30" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO30" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP30" t="s">
         <v>129</v>
       </c>
       <c r="AS30" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:45">
@@ -4523,20 +4784,23 @@
       <c r="AJ31" t="s">
         <v>135</v>
       </c>
+      <c r="AK31" t="s">
+        <v>165</v>
+      </c>
       <c r="AM31" t="s">
-        <v>167</v>
+        <v>227</v>
       </c>
       <c r="AN31" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO31" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP31" t="s">
         <v>129</v>
       </c>
       <c r="AS31" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:45">
@@ -4633,20 +4897,23 @@
       <c r="AJ32" t="s">
         <v>135</v>
       </c>
+      <c r="AK32" t="s">
+        <v>166</v>
+      </c>
       <c r="AM32" t="s">
-        <v>168</v>
+        <v>228</v>
       </c>
       <c r="AN32" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO32" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP32" t="s">
         <v>129</v>
       </c>
       <c r="AS32" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:45">
@@ -4743,20 +5010,23 @@
       <c r="AJ33" t="s">
         <v>135</v>
       </c>
+      <c r="AK33" t="s">
+        <v>167</v>
+      </c>
       <c r="AM33" t="s">
-        <v>169</v>
+        <v>229</v>
       </c>
       <c r="AN33" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO33" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP33" t="s">
         <v>129</v>
       </c>
       <c r="AS33" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:45">
@@ -4853,20 +5123,23 @@
       <c r="AJ34" t="s">
         <v>135</v>
       </c>
+      <c r="AK34" t="s">
+        <v>168</v>
+      </c>
       <c r="AM34" t="s">
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="AN34" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO34" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP34" t="s">
         <v>129</v>
       </c>
       <c r="AS34" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:45">
@@ -4963,20 +5236,23 @@
       <c r="AJ35" t="s">
         <v>135</v>
       </c>
+      <c r="AK35" t="s">
+        <v>169</v>
+      </c>
       <c r="AM35" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="AN35" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO35" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP35" t="s">
         <v>129</v>
       </c>
       <c r="AS35" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:45">
@@ -5073,20 +5349,23 @@
       <c r="AJ36" t="s">
         <v>135</v>
       </c>
+      <c r="AK36" t="s">
+        <v>170</v>
+      </c>
       <c r="AM36" t="s">
-        <v>172</v>
+        <v>232</v>
       </c>
       <c r="AN36" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO36" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP36" t="s">
         <v>129</v>
       </c>
       <c r="AS36" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:45">
@@ -5183,20 +5462,23 @@
       <c r="AJ37" t="s">
         <v>135</v>
       </c>
+      <c r="AK37" t="s">
+        <v>171</v>
+      </c>
       <c r="AM37" t="s">
-        <v>173</v>
+        <v>233</v>
       </c>
       <c r="AN37" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO37" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP37" t="s">
         <v>129</v>
       </c>
       <c r="AS37" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:45">
@@ -5293,20 +5575,23 @@
       <c r="AJ38" t="s">
         <v>135</v>
       </c>
+      <c r="AK38" t="s">
+        <v>172</v>
+      </c>
       <c r="AM38" t="s">
-        <v>174</v>
+        <v>234</v>
       </c>
       <c r="AN38" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO38" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP38" t="s">
         <v>129</v>
       </c>
       <c r="AS38" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:45">
@@ -5403,20 +5688,23 @@
       <c r="AJ39" t="s">
         <v>135</v>
       </c>
+      <c r="AK39" t="s">
+        <v>173</v>
+      </c>
       <c r="AM39" t="s">
-        <v>175</v>
+        <v>235</v>
       </c>
       <c r="AN39" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO39" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP39" t="s">
         <v>129</v>
       </c>
       <c r="AS39" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:45">
@@ -5507,20 +5795,23 @@
       <c r="AH40" t="s">
         <v>132</v>
       </c>
+      <c r="AK40" t="s">
+        <v>174</v>
+      </c>
       <c r="AM40" t="s">
-        <v>176</v>
+        <v>236</v>
       </c>
       <c r="AN40" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO40" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP40" t="s">
         <v>129</v>
       </c>
       <c r="AS40" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:45">
@@ -5611,20 +5902,23 @@
       <c r="AH41" t="s">
         <v>132</v>
       </c>
+      <c r="AK41" t="s">
+        <v>175</v>
+      </c>
       <c r="AM41" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="AN41" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO41" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP41" t="s">
         <v>129</v>
       </c>
       <c r="AS41" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:45">
@@ -5715,20 +6009,23 @@
       <c r="AH42" t="s">
         <v>132</v>
       </c>
+      <c r="AK42" t="s">
+        <v>176</v>
+      </c>
       <c r="AM42" t="s">
-        <v>178</v>
+        <v>238</v>
       </c>
       <c r="AN42" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO42" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP42" t="s">
         <v>129</v>
       </c>
       <c r="AS42" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:45">
@@ -5825,20 +6122,23 @@
       <c r="AJ43" t="s">
         <v>135</v>
       </c>
+      <c r="AK43" t="s">
+        <v>177</v>
+      </c>
       <c r="AM43" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="AN43" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO43" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP43" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="AS43" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:45">
@@ -5935,20 +6235,23 @@
       <c r="AJ44" t="s">
         <v>135</v>
       </c>
+      <c r="AK44" t="s">
+        <v>178</v>
+      </c>
       <c r="AM44" t="s">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="AN44" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO44" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP44" t="s">
         <v>129</v>
       </c>
       <c r="AS44" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:45">
@@ -6045,20 +6348,23 @@
       <c r="AJ45" t="s">
         <v>135</v>
       </c>
+      <c r="AK45" t="s">
+        <v>179</v>
+      </c>
       <c r="AM45" t="s">
-        <v>181</v>
+        <v>241</v>
       </c>
       <c r="AN45" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO45" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP45" t="s">
         <v>129</v>
       </c>
       <c r="AS45" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" spans="1:45">
@@ -6155,20 +6461,23 @@
       <c r="AJ46" t="s">
         <v>135</v>
       </c>
+      <c r="AK46" t="s">
+        <v>180</v>
+      </c>
       <c r="AM46" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="AN46" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO46" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP46" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="AS46" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:45">
@@ -6259,20 +6568,23 @@
       <c r="AH47" t="s">
         <v>132</v>
       </c>
+      <c r="AK47" t="s">
+        <v>181</v>
+      </c>
       <c r="AM47" t="s">
-        <v>183</v>
+        <v>243</v>
       </c>
       <c r="AN47" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO47" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP47" t="s">
         <v>129</v>
       </c>
       <c r="AS47" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:45">
@@ -6363,20 +6675,23 @@
       <c r="AH48" t="s">
         <v>132</v>
       </c>
+      <c r="AK48" t="s">
+        <v>182</v>
+      </c>
       <c r="AM48" t="s">
-        <v>184</v>
+        <v>244</v>
       </c>
       <c r="AN48" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO48" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP48" t="s">
         <v>129</v>
       </c>
       <c r="AS48" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:45">
@@ -6467,20 +6782,23 @@
       <c r="AH49" t="s">
         <v>132</v>
       </c>
+      <c r="AK49" t="s">
+        <v>183</v>
+      </c>
       <c r="AM49" t="s">
-        <v>185</v>
+        <v>245</v>
       </c>
       <c r="AN49" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO49" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP49" t="s">
         <v>129</v>
       </c>
       <c r="AS49" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50" spans="1:45">
@@ -6577,20 +6895,23 @@
       <c r="AJ50" t="s">
         <v>135</v>
       </c>
+      <c r="AK50" t="s">
+        <v>184</v>
+      </c>
       <c r="AM50" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="AN50" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO50" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP50" t="s">
         <v>129</v>
       </c>
       <c r="AS50" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51" spans="1:45">
@@ -6687,20 +7008,23 @@
       <c r="AJ51" t="s">
         <v>135</v>
       </c>
+      <c r="AK51" t="s">
+        <v>185</v>
+      </c>
       <c r="AM51" t="s">
-        <v>187</v>
+        <v>247</v>
       </c>
       <c r="AN51" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO51" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP51" t="s">
         <v>129</v>
       </c>
       <c r="AS51" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:45">
@@ -6797,14 +7121,17 @@
       <c r="AJ52" t="s">
         <v>135</v>
       </c>
+      <c r="AK52" t="s">
+        <v>186</v>
+      </c>
       <c r="AM52" t="s">
-        <v>188</v>
+        <v>248</v>
       </c>
       <c r="AN52" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AS52" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:45">
@@ -6901,20 +7228,23 @@
       <c r="AJ53" t="s">
         <v>135</v>
       </c>
+      <c r="AK53" t="s">
+        <v>187</v>
+      </c>
       <c r="AM53" t="s">
-        <v>189</v>
+        <v>249</v>
       </c>
       <c r="AN53" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO53" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP53" t="s">
         <v>129</v>
       </c>
       <c r="AS53" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:45">
@@ -7011,20 +7341,23 @@
       <c r="AJ54" t="s">
         <v>135</v>
       </c>
+      <c r="AK54" t="s">
+        <v>188</v>
+      </c>
       <c r="AM54" t="s">
-        <v>190</v>
+        <v>250</v>
       </c>
       <c r="AN54" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO54" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP54" t="s">
         <v>129</v>
       </c>
       <c r="AS54" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:45">
@@ -7121,20 +7454,23 @@
       <c r="AJ55" t="s">
         <v>135</v>
       </c>
+      <c r="AK55" t="s">
+        <v>189</v>
+      </c>
       <c r="AM55" t="s">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="AN55" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO55" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP55" t="s">
         <v>129</v>
       </c>
       <c r="AS55" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="56" spans="1:45">
@@ -7231,20 +7567,23 @@
       <c r="AJ56" t="s">
         <v>135</v>
       </c>
+      <c r="AK56" t="s">
+        <v>190</v>
+      </c>
       <c r="AM56" t="s">
-        <v>192</v>
+        <v>252</v>
       </c>
       <c r="AN56" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO56" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP56" t="s">
         <v>129</v>
       </c>
       <c r="AS56" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" spans="1:45">
@@ -7341,20 +7680,23 @@
       <c r="AJ57" t="s">
         <v>135</v>
       </c>
+      <c r="AK57" t="s">
+        <v>191</v>
+      </c>
       <c r="AM57" t="s">
-        <v>193</v>
+        <v>253</v>
       </c>
       <c r="AN57" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO57" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP57" t="s">
         <v>129</v>
       </c>
       <c r="AS57" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="58" spans="1:45">
@@ -7451,20 +7793,23 @@
       <c r="AJ58" t="s">
         <v>135</v>
       </c>
+      <c r="AK58" t="s">
+        <v>192</v>
+      </c>
       <c r="AM58" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="AN58" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO58" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP58" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="AS58" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:45">
@@ -7561,20 +7906,23 @@
       <c r="AJ59" t="s">
         <v>135</v>
       </c>
+      <c r="AK59" t="s">
+        <v>193</v>
+      </c>
       <c r="AM59" t="s">
-        <v>195</v>
+        <v>255</v>
       </c>
       <c r="AN59" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO59" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP59" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="AS59" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="60" spans="1:45">
@@ -7671,20 +8019,23 @@
       <c r="AJ60" t="s">
         <v>135</v>
       </c>
+      <c r="AK60" t="s">
+        <v>194</v>
+      </c>
       <c r="AM60" t="s">
-        <v>196</v>
+        <v>256</v>
       </c>
       <c r="AN60" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO60" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP60" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="AS60" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" spans="1:45">
@@ -7775,20 +8126,23 @@
       <c r="AH61" t="s">
         <v>132</v>
       </c>
+      <c r="AK61" t="s">
+        <v>195</v>
+      </c>
       <c r="AM61" t="s">
-        <v>197</v>
+        <v>257</v>
       </c>
       <c r="AN61" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO61" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP61" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="AS61" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="62" spans="1:45">
@@ -7885,17 +8239,20 @@
       <c r="AJ62" t="s">
         <v>135</v>
       </c>
+      <c r="AK62" t="s">
+        <v>196</v>
+      </c>
       <c r="AN62" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO62" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP62" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="AS62" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:45">
@@ -7992,20 +8349,23 @@
       <c r="AJ63" t="s">
         <v>135</v>
       </c>
+      <c r="AK63" t="s">
+        <v>197</v>
+      </c>
       <c r="AM63" t="s">
-        <v>198</v>
+        <v>258</v>
       </c>
       <c r="AN63" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="AO63" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="AP63" t="s">
         <v>129</v>
       </c>
       <c r="AS63" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -8087,13 +8447,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>203</v>
+        <v>263</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>264</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8101,10 +8461,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>266</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8112,10 +8472,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -8123,10 +8483,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -8134,10 +8494,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8145,10 +8505,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8156,10 +8516,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C7" t="s">
-        <v>213</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -8167,10 +8527,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -8178,10 +8538,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -8189,10 +8549,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -8200,10 +8560,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -8211,10 +8571,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -8222,10 +8582,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -8233,10 +8593,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C14" t="s">
-        <v>220</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -8244,10 +8604,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -8255,10 +8615,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -8266,10 +8626,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C17" t="s">
-        <v>223</v>
+        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -8277,10 +8637,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C18" t="s">
-        <v>224</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -8288,10 +8648,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C19" t="s">
-        <v>225</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -8299,10 +8659,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C20" t="s">
-        <v>226</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -8310,10 +8670,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C21" t="s">
-        <v>227</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -8321,10 +8681,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
-        <v>228</v>
+        <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -8332,10 +8692,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C23" t="s">
-        <v>229</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -8343,10 +8703,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C24" t="s">
-        <v>230</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -8354,10 +8714,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C25" t="s">
-        <v>231</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -8365,10 +8725,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C26" t="s">
-        <v>232</v>
+        <v>292</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -8376,10 +8736,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C27" t="s">
-        <v>233</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -8387,10 +8747,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C28" t="s">
-        <v>234</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -8398,10 +8758,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C29" t="s">
-        <v>235</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -8409,10 +8769,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C30" t="s">
-        <v>236</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -8420,10 +8780,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C31" t="s">
-        <v>237</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -8431,10 +8791,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C32" t="s">
-        <v>238</v>
+        <v>298</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -8442,10 +8802,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C33" t="s">
-        <v>239</v>
+        <v>299</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -8453,10 +8813,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C34" t="s">
-        <v>240</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -8464,10 +8824,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
+        <v>301</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -8475,10 +8835,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C36" t="s">
-        <v>242</v>
+        <v>302</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -8486,10 +8846,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C37" t="s">
-        <v>243</v>
+        <v>303</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -8497,10 +8857,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C38" t="s">
-        <v>244</v>
+        <v>304</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -8508,10 +8868,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C39" t="s">
-        <v>245</v>
+        <v>305</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -8519,10 +8879,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C40" t="s">
-        <v>246</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -8530,10 +8890,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C41" t="s">
-        <v>247</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -8541,10 +8901,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C42" t="s">
-        <v>248</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -8552,10 +8912,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C43" t="s">
-        <v>249</v>
+        <v>309</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -8563,10 +8923,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C44" t="s">
-        <v>250</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -8574,10 +8934,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C45" t="s">
-        <v>251</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -8585,10 +8945,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="C46" t="s">
-        <v>252</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating standardization for UVP projects
</commit_message>
<xml_diff>
--- a/raw/project_UVP_standardizer.xlsx
+++ b/raw/project_UVP_standardizer.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAEE99D-B057-114C-96D4-4115939B412F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="26660" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2318" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="248">
   <si>
     <t>Project_ID</t>
   </si>
@@ -425,189 +431,6 @@
     <t>object_annotation_status</t>
   </si>
   <si>
-    <t>uvp5_sn005_dewex_winter_2013</t>
-  </si>
-  <si>
-    <t>uvp5_sn003_dewex_spring_2013</t>
-  </si>
-  <si>
-    <t>uvp5_sn003_sargasso_a,uvp5_sn003_sargasso_b</t>
-  </si>
-  <si>
-    <t>uvp5_sn000_malina2009</t>
-  </si>
-  <si>
-    <t>uvp5_sn002_somba_ge_2014</t>
-  </si>
-  <si>
-    <t>uvp5_sn003_outpace_2015</t>
-  </si>
-  <si>
-    <t>uvp5_sn003_cassiopee_2015</t>
-  </si>
-  <si>
-    <t>uvp5_sn003_medsea2013</t>
-  </si>
-  <si>
-    <t>uvp5_sn000_operex2008</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2016_m130</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2017_fluxes1</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2016_m131</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2017_m135</t>
-  </si>
-  <si>
-    <t>uvp5_sn001_2013_m92</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2014_ps88b</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2014_m107</t>
-  </si>
-  <si>
-    <t>sn010_2015_m121</t>
-  </si>
-  <si>
-    <t>uvp5_sn001_2013_m93</t>
-  </si>
-  <si>
-    <t>uvp5_sn003_jerico_2017</t>
-  </si>
-  <si>
-    <t>uvp5_sn000_tara2009,uvp5_sn000_tara2010,uvp5_sn000_tara2011,uvp5_sn000_tara2012,uvp5_sn000_tara2013</t>
-  </si>
-  <si>
-    <t>uvp5_sn001_2012_msm23</t>
-  </si>
-  <si>
-    <t>uvp5_sn001_2013_m96</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2014_m108</t>
-  </si>
-  <si>
-    <t>uvp5_sn001_2014_msm40</t>
-  </si>
-  <si>
-    <t>uvp5_sn000_msm049</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2015_m116</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2015_m119</t>
-  </si>
-  <si>
-    <t>uvp5_sn001_2012_msm22</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2015_m120</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2014_m106</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2014_m105</t>
-  </si>
-  <si>
-    <t>uvp5_sn001_2013_m97</t>
-  </si>
-  <si>
-    <t>uvp4_sn001_2013_m98</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2017_m136</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2017_m137</t>
-  </si>
-  <si>
-    <t>uvp5_sn001_2017_m138</t>
-  </si>
-  <si>
-    <t>uvp5_sn003_iado_2017</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2017_fluxes2</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2014_eddy</t>
-  </si>
-  <si>
-    <t>uvp5_sn002_iado_2018</t>
-  </si>
-  <si>
-    <t>uvp5_sn210_2019_lima</t>
-  </si>
-  <si>
-    <t>uvp5_sn205_coastdark_2019</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2018_m147</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2018_m145</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2018_m148</t>
-  </si>
-  <si>
-    <t>uvp5_sn010_2016_love</t>
-  </si>
-  <si>
-    <t>uvp6_sn000110lp_2020_07_float_recover</t>
-  </si>
-  <si>
-    <t>uvp6_sn000006lp_2020_sc_basintest</t>
-  </si>
-  <si>
-    <t>uvp5_sn002_iado_2020</t>
-  </si>
-  <si>
-    <t>uvp6_sn000003lp_20201109_seaexplorer_002</t>
-  </si>
-  <si>
-    <t>uvp6_sn000125hf_20201022_rade_test_cdt</t>
-  </si>
-  <si>
-    <t>uvp5_sn205_so284_2021_filtered</t>
-  </si>
-  <si>
-    <t>uvp5_sn205_so285_2021_filtered</t>
-  </si>
-  <si>
-    <t>uvp5_sn003_tara_microbiome_2021</t>
-  </si>
-  <si>
-    <t>uvp6_sn000130hf_2021_amazomix</t>
-  </si>
-  <si>
-    <t>uvp5_sn210_2018_msm080</t>
-  </si>
-  <si>
-    <t>uvp5_sn210_2019_m158</t>
-  </si>
-  <si>
-    <t>uvp6_sn000130hf_202205_champlain_lake</t>
-  </si>
-  <si>
-    <t>uvp5_sn203_2022_so287</t>
-  </si>
-  <si>
-    <t>uvp5_sn203_2022_so288</t>
-  </si>
-  <si>
-    <t>uvp5_sn203_2022_so289</t>
-  </si>
-  <si>
     <t>acq_instrument</t>
   </si>
   <si>
@@ -768,13 +591,187 @@
   </si>
   <si>
     <t>Additional description of the sampling method or protocol (e.g. net_aperture:{field:net_surf,unit:square_meter}, fixative:{chemical:glutaraldehyde,concentration:0.1%}, reference: {https://doi.org/...,https://www.protocols.io/view/zooscan-protocol-yxmvmk8j9g3p/v1})</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>48;47</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>99;51;49;9;7;6</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>249</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>254</t>
+  </si>
+  <si>
+    <t>276</t>
+  </si>
+  <si>
+    <t>428</t>
+  </si>
+  <si>
+    <t>430</t>
+  </si>
+  <si>
+    <t>433</t>
+  </si>
+  <si>
+    <t>438</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>494</t>
+  </si>
+  <si>
+    <t>558</t>
+  </si>
+  <si>
+    <t>559</t>
+  </si>
+  <si>
+    <t>560</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,6 +847,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -896,7 +901,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -928,9 +933,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -962,6 +985,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1137,14 +1178,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AK43" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1281,7 +1331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1376,22 +1426,22 @@
         <v>135</v>
       </c>
       <c r="AM2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AN2" t="s">
         <v>136</v>
       </c>
-      <c r="AN2" t="s">
-        <v>197</v>
-      </c>
       <c r="AO2" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP2" t="s">
         <v>129</v>
       </c>
       <c r="AS2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1486,22 +1536,22 @@
         <v>135</v>
       </c>
       <c r="AM3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO3" t="s">
         <v>137</v>
       </c>
-      <c r="AN3" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>198</v>
-      </c>
       <c r="AP3" t="s">
         <v>129</v>
       </c>
       <c r="AS3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>22</v>
       </c>
@@ -1596,22 +1646,22 @@
         <v>135</v>
       </c>
       <c r="AM4" t="s">
-        <v>138</v>
+        <v>192</v>
       </c>
       <c r="AN4" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO4" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP4" t="s">
         <v>129</v>
       </c>
       <c r="AS4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>28</v>
       </c>
@@ -1706,16 +1756,16 @@
         <v>135</v>
       </c>
       <c r="AM5" t="s">
+        <v>193</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AS5" t="s">
         <v>139</v>
       </c>
-      <c r="AN5" t="s">
-        <v>197</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45">
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>36</v>
       </c>
@@ -1810,22 +1860,22 @@
         <v>135</v>
       </c>
       <c r="AM6" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
       <c r="AN6" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO6" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP6" t="s">
         <v>129</v>
       </c>
       <c r="AS6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>37</v>
       </c>
@@ -1920,22 +1970,22 @@
         <v>135</v>
       </c>
       <c r="AM7" t="s">
-        <v>141</v>
+        <v>195</v>
       </c>
       <c r="AN7" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO7" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP7" t="s">
         <v>129</v>
       </c>
       <c r="AS7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>38</v>
       </c>
@@ -2030,22 +2080,22 @@
         <v>135</v>
       </c>
       <c r="AM8" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="AN8" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO8" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP8" t="s">
         <v>129</v>
       </c>
       <c r="AS8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>39</v>
       </c>
@@ -2140,22 +2190,22 @@
         <v>135</v>
       </c>
       <c r="AM9" t="s">
-        <v>143</v>
+        <v>197</v>
       </c>
       <c r="AN9" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO9" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP9" t="s">
         <v>129</v>
       </c>
       <c r="AS9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>110</v>
       </c>
@@ -2250,22 +2300,22 @@
         <v>135</v>
       </c>
       <c r="AM10" t="s">
-        <v>144</v>
+        <v>198</v>
       </c>
       <c r="AN10" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO10" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP10" t="s">
         <v>129</v>
       </c>
       <c r="AS10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>214</v>
       </c>
@@ -2360,22 +2410,22 @@
         <v>135</v>
       </c>
       <c r="AM11" t="s">
-        <v>145</v>
+        <v>199</v>
       </c>
       <c r="AN11" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO11" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP11" t="s">
         <v>129</v>
       </c>
       <c r="AS11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>507</v>
       </c>
@@ -2470,22 +2520,22 @@
         <v>135</v>
       </c>
       <c r="AM12" t="s">
-        <v>146</v>
+        <v>200</v>
       </c>
       <c r="AN12" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO12" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP12" t="s">
         <v>129</v>
       </c>
       <c r="AS12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>545</v>
       </c>
@@ -2580,22 +2630,22 @@
         <v>135</v>
       </c>
       <c r="AM13" t="s">
-        <v>147</v>
+        <v>201</v>
       </c>
       <c r="AN13" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO13" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP13" t="s">
         <v>129</v>
       </c>
       <c r="AS13" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>548</v>
       </c>
@@ -2690,22 +2740,22 @@
         <v>135</v>
       </c>
       <c r="AM14" t="s">
-        <v>148</v>
+        <v>202</v>
       </c>
       <c r="AN14" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO14" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP14" t="s">
         <v>129</v>
       </c>
       <c r="AS14" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>556</v>
       </c>
@@ -2800,16 +2850,16 @@
         <v>135</v>
       </c>
       <c r="AM15" t="s">
-        <v>149</v>
+        <v>203</v>
       </c>
       <c r="AN15" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>558</v>
       </c>
@@ -2904,16 +2954,16 @@
         <v>135</v>
       </c>
       <c r="AM16" t="s">
-        <v>150</v>
+        <v>204</v>
       </c>
       <c r="AN16" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>559</v>
       </c>
@@ -3008,22 +3058,22 @@
         <v>135</v>
       </c>
       <c r="AM17" t="s">
-        <v>151</v>
+        <v>205</v>
       </c>
       <c r="AN17" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO17" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP17" t="s">
         <v>129</v>
       </c>
       <c r="AS17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>560</v>
       </c>
@@ -3117,23 +3167,23 @@
       <c r="AJ18" t="s">
         <v>135</v>
       </c>
-      <c r="AM18" t="s">
-        <v>152</v>
+      <c r="AM18">
+        <v>76</v>
       </c>
       <c r="AN18" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO18" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP18" t="s">
         <v>129</v>
       </c>
       <c r="AS18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>563</v>
       </c>
@@ -3228,22 +3278,22 @@
         <v>135</v>
       </c>
       <c r="AM19" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="AN19" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO19" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP19" t="s">
         <v>129</v>
       </c>
       <c r="AS19" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>578</v>
       </c>
@@ -3338,22 +3388,22 @@
         <v>135</v>
       </c>
       <c r="AM20" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
       <c r="AN20" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO20" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP20" t="s">
         <v>129</v>
       </c>
       <c r="AS20" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>579</v>
       </c>
@@ -3448,22 +3498,22 @@
         <v>135</v>
       </c>
       <c r="AM21" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="AN21" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO21" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP21" t="s">
         <v>129</v>
       </c>
       <c r="AS21" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>584</v>
       </c>
@@ -3558,22 +3608,22 @@
         <v>135</v>
       </c>
       <c r="AM22" t="s">
-        <v>156</v>
+        <v>209</v>
       </c>
       <c r="AN22" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO22" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP22" t="s">
         <v>129</v>
       </c>
       <c r="AS22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>585</v>
       </c>
@@ -3668,16 +3718,16 @@
         <v>135</v>
       </c>
       <c r="AM23" t="s">
-        <v>157</v>
+        <v>210</v>
       </c>
       <c r="AN23" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS23" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>586</v>
       </c>
@@ -3772,22 +3822,22 @@
         <v>135</v>
       </c>
       <c r="AM24" t="s">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="AN24" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO24" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP24" t="s">
         <v>129</v>
       </c>
       <c r="AS24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>587</v>
       </c>
@@ -3882,16 +3932,16 @@
         <v>135</v>
       </c>
       <c r="AM25" t="s">
-        <v>159</v>
+        <v>212</v>
       </c>
       <c r="AN25" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS25" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>588</v>
       </c>
@@ -3986,22 +4036,22 @@
         <v>135</v>
       </c>
       <c r="AM26" t="s">
-        <v>160</v>
+        <v>213</v>
       </c>
       <c r="AN26" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO26" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP26" t="s">
         <v>129</v>
       </c>
       <c r="AS26" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>589</v>
       </c>
@@ -4096,22 +4146,22 @@
         <v>135</v>
       </c>
       <c r="AM27" t="s">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="AN27" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO27" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP27" t="s">
         <v>129</v>
       </c>
       <c r="AS27" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>590</v>
       </c>
@@ -4206,22 +4256,22 @@
         <v>135</v>
       </c>
       <c r="AM28" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
       <c r="AN28" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO28" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP28" t="s">
         <v>129</v>
       </c>
       <c r="AS28" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="29" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>593</v>
       </c>
@@ -4316,16 +4366,16 @@
         <v>135</v>
       </c>
       <c r="AM29" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="AN29" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS29" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>594</v>
       </c>
@@ -4420,22 +4470,22 @@
         <v>135</v>
       </c>
       <c r="AM30" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="AN30" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO30" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP30" t="s">
         <v>129</v>
       </c>
       <c r="AS30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>595</v>
       </c>
@@ -4530,22 +4580,22 @@
         <v>135</v>
       </c>
       <c r="AM31" t="s">
-        <v>165</v>
+        <v>218</v>
       </c>
       <c r="AN31" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO31" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP31" t="s">
         <v>129</v>
       </c>
       <c r="AS31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="32" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>602</v>
       </c>
@@ -4640,16 +4690,16 @@
         <v>135</v>
       </c>
       <c r="AM32" t="s">
-        <v>166</v>
+        <v>219</v>
       </c>
       <c r="AN32" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS32" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="33" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>603</v>
       </c>
@@ -4744,16 +4794,16 @@
         <v>135</v>
       </c>
       <c r="AM33" t="s">
-        <v>167</v>
+        <v>220</v>
       </c>
       <c r="AN33" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS33" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>610</v>
       </c>
@@ -4848,16 +4898,16 @@
         <v>135</v>
       </c>
       <c r="AM34" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
       <c r="AN34" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS34" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="35" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>620</v>
       </c>
@@ -4952,22 +5002,22 @@
         <v>135</v>
       </c>
       <c r="AM35" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="AN35" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO35" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP35" t="s">
         <v>129</v>
       </c>
       <c r="AS35" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="36" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>621</v>
       </c>
@@ -5062,22 +5112,22 @@
         <v>135</v>
       </c>
       <c r="AM36" t="s">
-        <v>170</v>
+        <v>223</v>
       </c>
       <c r="AN36" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO36" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP36" t="s">
         <v>129</v>
       </c>
       <c r="AS36" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="37" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>622</v>
       </c>
@@ -5172,16 +5222,16 @@
         <v>135</v>
       </c>
       <c r="AM37" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="AN37" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AS37" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>651</v>
       </c>
@@ -5276,22 +5326,22 @@
         <v>135</v>
       </c>
       <c r="AM38" t="s">
-        <v>172</v>
+        <v>225</v>
       </c>
       <c r="AN38" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO38" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP38" t="s">
         <v>129</v>
       </c>
       <c r="AS38" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>855</v>
       </c>
@@ -5386,22 +5436,22 @@
         <v>135</v>
       </c>
       <c r="AM39" t="s">
-        <v>173</v>
+        <v>226</v>
       </c>
       <c r="AN39" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO39" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP39" t="s">
         <v>129</v>
       </c>
       <c r="AS39" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="40" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>881</v>
       </c>
@@ -5496,22 +5546,22 @@
         <v>135</v>
       </c>
       <c r="AM40" t="s">
-        <v>174</v>
+        <v>227</v>
       </c>
       <c r="AN40" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO40" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP40" t="s">
         <v>129</v>
       </c>
       <c r="AS40" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="41" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1343</v>
       </c>
@@ -5606,22 +5656,22 @@
         <v>135</v>
       </c>
       <c r="AM41" t="s">
-        <v>175</v>
+        <v>228</v>
       </c>
       <c r="AN41" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO41" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP41" t="s">
         <v>129</v>
       </c>
       <c r="AS41" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2465</v>
       </c>
@@ -5716,22 +5766,22 @@
         <v>135</v>
       </c>
       <c r="AM42" t="s">
-        <v>176</v>
+        <v>229</v>
       </c>
       <c r="AN42" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO42" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP42" t="s">
         <v>129</v>
       </c>
       <c r="AS42" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2483</v>
       </c>
@@ -5826,22 +5876,22 @@
         <v>135</v>
       </c>
       <c r="AM43" t="s">
-        <v>177</v>
+        <v>230</v>
       </c>
       <c r="AN43" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO43" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP43" t="s">
         <v>129</v>
       </c>
       <c r="AS43" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2806</v>
       </c>
@@ -5936,22 +5986,22 @@
         <v>135</v>
       </c>
       <c r="AM44" t="s">
-        <v>178</v>
+        <v>231</v>
       </c>
       <c r="AN44" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO44" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP44" t="s">
         <v>129</v>
       </c>
       <c r="AS44" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2807</v>
       </c>
@@ -6046,22 +6096,22 @@
         <v>135</v>
       </c>
       <c r="AM45" t="s">
-        <v>179</v>
+        <v>232</v>
       </c>
       <c r="AN45" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO45" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP45" t="s">
         <v>129</v>
       </c>
       <c r="AS45" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2808</v>
       </c>
@@ -6156,22 +6206,22 @@
         <v>135</v>
       </c>
       <c r="AM46" t="s">
-        <v>180</v>
+        <v>233</v>
       </c>
       <c r="AN46" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO46" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP46" t="s">
         <v>129</v>
       </c>
       <c r="AS46" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3117</v>
       </c>
@@ -6266,22 +6316,22 @@
         <v>135</v>
       </c>
       <c r="AM47" t="s">
-        <v>181</v>
+        <v>234</v>
       </c>
       <c r="AN47" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO47" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP47" t="s">
         <v>129</v>
       </c>
       <c r="AS47" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="48" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3278</v>
       </c>
@@ -6376,22 +6426,22 @@
         <v>135</v>
       </c>
       <c r="AM48" t="s">
-        <v>182</v>
+        <v>235</v>
       </c>
       <c r="AN48" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO48" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP48" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="AS48" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="49" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3327</v>
       </c>
@@ -6486,22 +6536,22 @@
         <v>135</v>
       </c>
       <c r="AM49" t="s">
-        <v>183</v>
+        <v>236</v>
       </c>
       <c r="AN49" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO49" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP49" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="AS49" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3403</v>
       </c>
@@ -6590,22 +6640,22 @@
         <v>132</v>
       </c>
       <c r="AM50" t="s">
-        <v>184</v>
+        <v>237</v>
       </c>
       <c r="AN50" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO50" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP50" t="s">
         <v>129</v>
       </c>
       <c r="AS50" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3887</v>
       </c>
@@ -6700,22 +6750,22 @@
         <v>135</v>
       </c>
       <c r="AM51" t="s">
-        <v>185</v>
+        <v>238</v>
       </c>
       <c r="AN51" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO51" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP51" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="AS51" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3943</v>
       </c>
@@ -6803,23 +6853,23 @@
       <c r="AH52" t="s">
         <v>133</v>
       </c>
-      <c r="AM52" t="s">
-        <v>186</v>
+      <c r="AM52">
+        <v>284</v>
       </c>
       <c r="AN52" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO52" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP52" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="AS52" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="53" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>4591</v>
       </c>
@@ -6914,19 +6964,19 @@
         <v>135</v>
       </c>
       <c r="AN53" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO53" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP53" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="AS53" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="54" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>5197</v>
       </c>
@@ -7015,22 +7065,22 @@
         <v>132</v>
       </c>
       <c r="AM54" t="s">
-        <v>187</v>
+        <v>239</v>
       </c>
       <c r="AN54" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO54" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP54" t="s">
         <v>129</v>
       </c>
       <c r="AS54" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="55" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>5208</v>
       </c>
@@ -7119,22 +7169,22 @@
         <v>132</v>
       </c>
       <c r="AM55" t="s">
-        <v>188</v>
+        <v>240</v>
       </c>
       <c r="AN55" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO55" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP55" t="s">
         <v>129</v>
       </c>
       <c r="AS55" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="56" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5254</v>
       </c>
@@ -7229,22 +7279,22 @@
         <v>135</v>
       </c>
       <c r="AM56" t="s">
-        <v>189</v>
+        <v>241</v>
       </c>
       <c r="AN56" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO56" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP56" t="s">
         <v>129</v>
       </c>
       <c r="AS56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="57" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>5680</v>
       </c>
@@ -7339,22 +7389,22 @@
         <v>135</v>
       </c>
       <c r="AM57" t="s">
-        <v>190</v>
+        <v>242</v>
       </c>
       <c r="AN57" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO57" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP57" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="AS57" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="58" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>5690</v>
       </c>
@@ -7448,23 +7498,23 @@
       <c r="AJ58" t="s">
         <v>135</v>
       </c>
-      <c r="AM58" t="s">
-        <v>191</v>
+      <c r="AM58">
+        <v>270</v>
       </c>
       <c r="AN58" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO58" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP58" t="s">
         <v>129</v>
       </c>
       <c r="AS58" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="59" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>5693</v>
       </c>
@@ -7559,22 +7609,22 @@
         <v>135</v>
       </c>
       <c r="AM59" t="s">
-        <v>192</v>
+        <v>243</v>
       </c>
       <c r="AN59" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO59" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP59" t="s">
         <v>129</v>
       </c>
       <c r="AS59" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="60" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>6047</v>
       </c>
@@ -7669,22 +7719,22 @@
         <v>135</v>
       </c>
       <c r="AM60" t="s">
-        <v>193</v>
+        <v>244</v>
       </c>
       <c r="AN60" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO60" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP60" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="AS60" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="61" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>6702</v>
       </c>
@@ -7773,22 +7823,22 @@
         <v>132</v>
       </c>
       <c r="AM61" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="AN61" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO61" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP61" t="s">
         <v>129</v>
       </c>
       <c r="AS61" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="62" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>6703</v>
       </c>
@@ -7877,22 +7927,22 @@
         <v>132</v>
       </c>
       <c r="AM62" t="s">
-        <v>195</v>
+        <v>246</v>
       </c>
       <c r="AN62" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO62" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP62" t="s">
         <v>129</v>
       </c>
       <c r="AS62" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="63" spans="1:45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>6704</v>
       </c>
@@ -7981,602 +8031,602 @@
         <v>132</v>
       </c>
       <c r="AM63" t="s">
-        <v>196</v>
+        <v>247</v>
       </c>
       <c r="AN63" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="AO63" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="AP63" t="s">
         <v>129</v>
       </c>
       <c r="AS63" t="s">
-        <v>200</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
-    <hyperlink ref="B30" r:id="rId29"/>
-    <hyperlink ref="B31" r:id="rId30"/>
-    <hyperlink ref="B32" r:id="rId31"/>
-    <hyperlink ref="B33" r:id="rId32"/>
-    <hyperlink ref="B34" r:id="rId33"/>
-    <hyperlink ref="B35" r:id="rId34"/>
-    <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B37" r:id="rId36"/>
-    <hyperlink ref="B38" r:id="rId37"/>
-    <hyperlink ref="B39" r:id="rId38"/>
-    <hyperlink ref="B40" r:id="rId39"/>
-    <hyperlink ref="B41" r:id="rId40"/>
-    <hyperlink ref="B42" r:id="rId41"/>
-    <hyperlink ref="B43" r:id="rId42"/>
-    <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
-    <hyperlink ref="B46" r:id="rId45"/>
-    <hyperlink ref="B47" r:id="rId46"/>
-    <hyperlink ref="B48" r:id="rId47"/>
-    <hyperlink ref="B49" r:id="rId48"/>
-    <hyperlink ref="B50" r:id="rId49"/>
-    <hyperlink ref="B51" r:id="rId50"/>
-    <hyperlink ref="B52" r:id="rId51"/>
-    <hyperlink ref="B53" r:id="rId52"/>
-    <hyperlink ref="B54" r:id="rId53"/>
-    <hyperlink ref="B55" r:id="rId54"/>
-    <hyperlink ref="B56" r:id="rId55"/>
-    <hyperlink ref="B57" r:id="rId56"/>
-    <hyperlink ref="B58" r:id="rId57"/>
-    <hyperlink ref="B59" r:id="rId58"/>
-    <hyperlink ref="B60" r:id="rId59"/>
-    <hyperlink ref="B61" r:id="rId60"/>
-    <hyperlink ref="B62" r:id="rId61"/>
-    <hyperlink ref="B63" r:id="rId62"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C20" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C21" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C26" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C30" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C32" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C33" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C35" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C38" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C40" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C41" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C43" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C44" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C45" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C46" t="s">
-        <v>250</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing UVP project ok
</commit_message>
<xml_diff>
--- a/raw/project_UVP_standardizer.xlsx
+++ b/raw/project_UVP_standardizer.xlsx
@@ -1111,7 +1111,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_4_flags.csv</t>
+        </is>
+      </c>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr">
         <is>
@@ -1300,7 +1304,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_22_flags.csv</t>
+        </is>
+      </c>
       <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="inlineStr">
         <is>
@@ -1489,7 +1497,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_28_flags.csv</t>
+        </is>
+      </c>
       <c r="AL5" t="inlineStr"/>
       <c r="AM5" t="inlineStr">
         <is>
@@ -1670,7 +1682,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_36_flags.csv</t>
+        </is>
+      </c>
       <c r="AL6" t="inlineStr"/>
       <c r="AM6" t="inlineStr">
         <is>
@@ -1859,7 +1875,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_37_flags.csv</t>
+        </is>
+      </c>
       <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="inlineStr">
         <is>
@@ -2048,7 +2068,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_38_flags.csv</t>
+        </is>
+      </c>
       <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="inlineStr">
         <is>
@@ -2615,7 +2639,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_110_flags.csv</t>
+        </is>
+      </c>
       <c r="AL11" t="inlineStr"/>
       <c r="AM11" t="inlineStr">
         <is>
@@ -2993,7 +3021,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_507_flags.csv</t>
+        </is>
+      </c>
       <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="inlineStr">
         <is>
@@ -3371,7 +3403,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK15" t="inlineStr"/>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_548_flags.csv</t>
+        </is>
+      </c>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr">
         <is>
@@ -3560,7 +3596,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK16" t="inlineStr"/>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_556_flags.csv</t>
+        </is>
+      </c>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr">
         <is>
@@ -3741,7 +3781,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK17" t="inlineStr"/>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_558_flags.csv</t>
+        </is>
+      </c>
       <c r="AL17" t="inlineStr"/>
       <c r="AM17" t="inlineStr">
         <is>
@@ -3922,7 +3966,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK18" t="inlineStr"/>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_559_flags.csv</t>
+        </is>
+      </c>
       <c r="AL18" t="inlineStr"/>
       <c r="AM18" t="inlineStr">
         <is>
@@ -4111,7 +4159,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK19" t="inlineStr"/>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_560_flags.csv</t>
+        </is>
+      </c>
       <c r="AL19" t="inlineStr"/>
       <c r="AM19" t="n">
         <v>76</v>
@@ -4298,7 +4350,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK20" t="inlineStr"/>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_563_flags.csv</t>
+        </is>
+      </c>
       <c r="AL20" t="inlineStr"/>
       <c r="AM20" t="inlineStr">
         <is>
@@ -4487,7 +4543,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK21" t="inlineStr"/>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_578_flags.csv</t>
+        </is>
+      </c>
       <c r="AL21" t="inlineStr"/>
       <c r="AM21" t="inlineStr">
         <is>
@@ -4676,7 +4736,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK22" t="inlineStr"/>
+      <c r="AK22" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_579_flags.csv</t>
+        </is>
+      </c>
       <c r="AL22" t="inlineStr"/>
       <c r="AM22" t="inlineStr">
         <is>
@@ -4865,7 +4929,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK23" t="inlineStr"/>
+      <c r="AK23" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_584_flags.csv</t>
+        </is>
+      </c>
       <c r="AL23" t="inlineStr"/>
       <c r="AM23" t="inlineStr">
         <is>
@@ -5054,7 +5122,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK24" t="inlineStr"/>
+      <c r="AK24" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_585_flags.csv</t>
+        </is>
+      </c>
       <c r="AL24" t="inlineStr"/>
       <c r="AM24" t="inlineStr">
         <is>
@@ -5235,7 +5307,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK25" t="inlineStr"/>
+      <c r="AK25" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_586_flags.csv</t>
+        </is>
+      </c>
       <c r="AL25" t="inlineStr"/>
       <c r="AM25" t="inlineStr">
         <is>
@@ -5424,7 +5500,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK26" t="inlineStr"/>
+      <c r="AK26" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_587_flags.csv</t>
+        </is>
+      </c>
       <c r="AL26" t="inlineStr"/>
       <c r="AM26" t="inlineStr">
         <is>
@@ -5605,7 +5685,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK27" t="inlineStr"/>
+      <c r="AK27" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_588_flags.csv</t>
+        </is>
+      </c>
       <c r="AL27" t="inlineStr"/>
       <c r="AM27" t="inlineStr">
         <is>
@@ -5794,7 +5878,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK28" t="inlineStr"/>
+      <c r="AK28" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_589_flags.csv</t>
+        </is>
+      </c>
       <c r="AL28" t="inlineStr"/>
       <c r="AM28" t="inlineStr">
         <is>
@@ -5983,7 +6071,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK29" t="inlineStr"/>
+      <c r="AK29" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_590_flags.csv</t>
+        </is>
+      </c>
       <c r="AL29" t="inlineStr"/>
       <c r="AM29" t="inlineStr">
         <is>
@@ -6172,7 +6264,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK30" t="inlineStr"/>
+      <c r="AK30" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_593_flags.csv</t>
+        </is>
+      </c>
       <c r="AL30" t="inlineStr"/>
       <c r="AM30" t="inlineStr">
         <is>
@@ -6353,7 +6449,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK31" t="inlineStr"/>
+      <c r="AK31" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_594_flags.csv</t>
+        </is>
+      </c>
       <c r="AL31" t="inlineStr"/>
       <c r="AM31" t="inlineStr">
         <is>
@@ -6542,7 +6642,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK32" t="inlineStr"/>
+      <c r="AK32" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_595_flags.csv</t>
+        </is>
+      </c>
       <c r="AL32" t="inlineStr"/>
       <c r="AM32" t="inlineStr">
         <is>
@@ -6731,7 +6835,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK33" t="inlineStr"/>
+      <c r="AK33" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_602_flags.csv</t>
+        </is>
+      </c>
       <c r="AL33" t="inlineStr"/>
       <c r="AM33" t="inlineStr">
         <is>
@@ -6912,7 +7020,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK34" t="inlineStr"/>
+      <c r="AK34" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_603_flags.csv</t>
+        </is>
+      </c>
       <c r="AL34" t="inlineStr"/>
       <c r="AM34" t="inlineStr">
         <is>
@@ -7093,7 +7205,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK35" t="inlineStr"/>
+      <c r="AK35" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_610_flags.csv</t>
+        </is>
+      </c>
       <c r="AL35" t="inlineStr"/>
       <c r="AM35" t="inlineStr">
         <is>
@@ -7274,7 +7390,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK36" t="inlineStr"/>
+      <c r="AK36" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_620_flags.csv</t>
+        </is>
+      </c>
       <c r="AL36" t="inlineStr"/>
       <c r="AM36" t="inlineStr">
         <is>
@@ -7652,7 +7772,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK38" t="inlineStr"/>
+      <c r="AK38" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_622_flags.csv</t>
+        </is>
+      </c>
       <c r="AL38" t="inlineStr"/>
       <c r="AM38" t="inlineStr">
         <is>
@@ -7833,7 +7957,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK39" t="inlineStr"/>
+      <c r="AK39" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_651_flags.csv</t>
+        </is>
+      </c>
       <c r="AL39" t="inlineStr"/>
       <c r="AM39" t="inlineStr">
         <is>
@@ -8022,7 +8150,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK40" t="inlineStr"/>
+      <c r="AK40" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_855_flags.csv</t>
+        </is>
+      </c>
       <c r="AL40" t="inlineStr"/>
       <c r="AM40" t="inlineStr">
         <is>
@@ -8211,7 +8343,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK41" t="inlineStr"/>
+      <c r="AK41" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_881_flags.csv</t>
+        </is>
+      </c>
       <c r="AL41" t="inlineStr"/>
       <c r="AM41" t="inlineStr">
         <is>
@@ -8400,7 +8536,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK42" t="inlineStr"/>
+      <c r="AK42" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_1343_flags.csv</t>
+        </is>
+      </c>
       <c r="AL42" t="inlineStr"/>
       <c r="AM42" t="inlineStr">
         <is>
@@ -8967,7 +9107,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK45" t="inlineStr"/>
+      <c r="AK45" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_2465_flags.csv</t>
+        </is>
+      </c>
       <c r="AL45" t="inlineStr"/>
       <c r="AM45" t="inlineStr">
         <is>
@@ -9156,7 +9300,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK46" t="inlineStr"/>
+      <c r="AK46" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_2483_flags.csv</t>
+        </is>
+      </c>
       <c r="AL46" t="inlineStr"/>
       <c r="AM46" t="inlineStr">
         <is>
@@ -9345,7 +9493,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK47" t="inlineStr"/>
+      <c r="AK47" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_2806_flags.csv</t>
+        </is>
+      </c>
       <c r="AL47" t="inlineStr"/>
       <c r="AM47" t="inlineStr">
         <is>
@@ -9534,7 +9686,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK48" t="inlineStr"/>
+      <c r="AK48" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_2807_flags.csv</t>
+        </is>
+      </c>
       <c r="AL48" t="inlineStr"/>
       <c r="AM48" t="inlineStr">
         <is>
@@ -9723,7 +9879,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK49" t="inlineStr"/>
+      <c r="AK49" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_2808_flags.csv</t>
+        </is>
+      </c>
       <c r="AL49" t="inlineStr"/>
       <c r="AM49" t="inlineStr">
         <is>
@@ -9912,7 +10072,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK50" t="inlineStr"/>
+      <c r="AK50" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_3117_flags.csv</t>
+        </is>
+      </c>
       <c r="AL50" t="inlineStr"/>
       <c r="AM50" t="inlineStr">
         <is>
@@ -10101,7 +10265,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK51" t="inlineStr"/>
+      <c r="AK51" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_3278_flags.csv</t>
+        </is>
+      </c>
       <c r="AL51" t="inlineStr"/>
       <c r="AM51" t="inlineStr">
         <is>
@@ -10290,7 +10458,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK52" t="inlineStr"/>
+      <c r="AK52" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_3327_flags.csv</t>
+        </is>
+      </c>
       <c r="AL52" t="inlineStr"/>
       <c r="AM52" t="inlineStr">
         <is>
@@ -10471,7 +10643,11 @@
       </c>
       <c r="AI53" t="inlineStr"/>
       <c r="AJ53" t="inlineStr"/>
-      <c r="AK53" t="inlineStr"/>
+      <c r="AK53" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_3403_flags.csv</t>
+        </is>
+      </c>
       <c r="AL53" t="inlineStr"/>
       <c r="AM53" t="inlineStr">
         <is>
@@ -10660,7 +10836,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK54" t="inlineStr"/>
+      <c r="AK54" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_3887_flags.csv</t>
+        </is>
+      </c>
       <c r="AL54" t="inlineStr"/>
       <c r="AM54" t="inlineStr">
         <is>
@@ -10841,7 +11021,11 @@
       </c>
       <c r="AI55" t="inlineStr"/>
       <c r="AJ55" t="inlineStr"/>
-      <c r="AK55" t="inlineStr"/>
+      <c r="AK55" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_3943_flags.csv</t>
+        </is>
+      </c>
       <c r="AL55" t="inlineStr"/>
       <c r="AM55" t="n">
         <v>284</v>
@@ -11028,7 +11212,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK56" t="inlineStr"/>
+      <c r="AK56" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_4591_flags.csv</t>
+        </is>
+      </c>
       <c r="AL56" t="inlineStr"/>
       <c r="AM56" t="inlineStr"/>
       <c r="AN56" t="inlineStr">
@@ -11205,7 +11393,11 @@
       </c>
       <c r="AI57" t="inlineStr"/>
       <c r="AJ57" t="inlineStr"/>
-      <c r="AK57" t="inlineStr"/>
+      <c r="AK57" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_5197_flags.csv</t>
+        </is>
+      </c>
       <c r="AL57" t="inlineStr"/>
       <c r="AM57" t="inlineStr">
         <is>
@@ -11386,7 +11578,11 @@
       </c>
       <c r="AI58" t="inlineStr"/>
       <c r="AJ58" t="inlineStr"/>
-      <c r="AK58" t="inlineStr"/>
+      <c r="AK58" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_5208_flags.csv</t>
+        </is>
+      </c>
       <c r="AL58" t="inlineStr"/>
       <c r="AM58" t="inlineStr">
         <is>
@@ -11575,7 +11771,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK59" t="inlineStr"/>
+      <c r="AK59" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_5254_flags.csv</t>
+        </is>
+      </c>
       <c r="AL59" t="inlineStr"/>
       <c r="AM59" t="inlineStr">
         <is>
@@ -11764,7 +11964,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK60" t="inlineStr"/>
+      <c r="AK60" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_5680_flags.csv</t>
+        </is>
+      </c>
       <c r="AL60" t="inlineStr"/>
       <c r="AM60" t="inlineStr">
         <is>
@@ -11953,7 +12157,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK61" t="inlineStr"/>
+      <c r="AK61" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_5690_flags.csv</t>
+        </is>
+      </c>
       <c r="AL61" t="inlineStr"/>
       <c r="AM61" t="n">
         <v>270</v>
@@ -12329,7 +12537,11 @@
           <t>object_annotation_status</t>
         </is>
       </c>
-      <c r="AK63" t="inlineStr"/>
+      <c r="AK63" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6047_flags.csv</t>
+        </is>
+      </c>
       <c r="AL63" t="inlineStr"/>
       <c r="AM63" t="inlineStr">
         <is>
@@ -12510,7 +12722,11 @@
       </c>
       <c r="AI64" t="inlineStr"/>
       <c r="AJ64" t="inlineStr"/>
-      <c r="AK64" t="inlineStr"/>
+      <c r="AK64" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6702_flags.csv</t>
+        </is>
+      </c>
       <c r="AL64" t="inlineStr"/>
       <c r="AM64" t="inlineStr">
         <is>
@@ -12691,7 +12907,11 @@
       </c>
       <c r="AI65" t="inlineStr"/>
       <c r="AJ65" t="inlineStr"/>
-      <c r="AK65" t="inlineStr"/>
+      <c r="AK65" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6703_flags.csv</t>
+        </is>
+      </c>
       <c r="AL65" t="inlineStr"/>
       <c r="AM65" t="inlineStr">
         <is>
@@ -12872,7 +13092,11 @@
       </c>
       <c r="AI66" t="inlineStr"/>
       <c r="AJ66" t="inlineStr"/>
-      <c r="AK66" t="inlineStr"/>
+      <c r="AK66" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6704_flags.csv</t>
+        </is>
+      </c>
       <c r="AL66" t="inlineStr"/>
       <c r="AM66" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Allowing for UVP projects consolidation if native project folder is missing or messy
</commit_message>
<xml_diff>
--- a/raw/project_UVP_standardizer.xlsx
+++ b/raw/project_UVP_standardizer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65EF5D2-6A13-584B-81E5-E9E9906CC5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814BC9A2-DE56-4E44-BAA3-DF99ADFE908B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="25940" windowHeight="11940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="25940" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecotaxa" sheetId="1" r:id="rId1"/>
@@ -2448,11 +2448,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS66"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2:AK66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -9645,8 +9648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S241" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:AI244"/>
+    <sheetView topLeftCell="S241" workbookViewId="0">
+      <selection activeCell="U253" sqref="U253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Re-processing UVP projects 29 and 545 for the data release
</commit_message>
<xml_diff>
--- a/raw/project_UVP_standardizer.xlsx
+++ b/raw/project_UVP_standardizer.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -54,6 +54,12 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -65,12 +71,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -129,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -142,6 +163,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -555,227 +579,227 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Project_ID</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Project_source</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Project_localpath</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Instrument</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Cruise_field</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>Station_field</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
         <is>
           <t>Profile_field</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="6" t="inlineStr">
         <is>
           <t>Sample_field</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="6" t="inlineStr">
         <is>
           <t>Latitude_field</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="6" t="inlineStr">
         <is>
           <t>Latitude_unit</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="6" t="inlineStr">
         <is>
           <t>Longitude_field</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="6" t="inlineStr">
         <is>
           <t>Longitude_unit</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="6" t="inlineStr">
         <is>
           <t>Depth_min_field</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="6" t="inlineStr">
         <is>
           <t>Depth_min_unit</t>
         </is>
       </c>
-      <c r="O1" s="5" t="inlineStr">
+      <c r="O1" s="6" t="inlineStr">
         <is>
           <t>Depth_max_field</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="P1" s="6" t="inlineStr">
         <is>
           <t>Depth_max_unit</t>
         </is>
       </c>
-      <c r="Q1" s="5" t="inlineStr">
+      <c r="Q1" s="6" t="inlineStr">
         <is>
           <t>Sampling_date_field</t>
         </is>
       </c>
-      <c r="R1" s="5" t="inlineStr">
+      <c r="R1" s="6" t="inlineStr">
         <is>
           <t>Sampling_date_format</t>
         </is>
       </c>
-      <c r="S1" s="5" t="inlineStr">
+      <c r="S1" s="6" t="inlineStr">
         <is>
           <t>Sampling_time_field</t>
         </is>
       </c>
-      <c r="T1" s="5" t="inlineStr">
+      <c r="T1" s="6" t="inlineStr">
         <is>
           <t>Sampling_time_format</t>
         </is>
       </c>
-      <c r="U1" s="5" t="inlineStr">
+      <c r="U1" s="6" t="inlineStr">
         <is>
           <t>Volume_analyzed_field</t>
         </is>
       </c>
-      <c r="V1" s="5" t="inlineStr">
+      <c r="V1" s="6" t="inlineStr">
         <is>
           <t>Volume_analyzed_unit</t>
         </is>
       </c>
-      <c r="W1" s="5" t="inlineStr">
+      <c r="W1" s="6" t="inlineStr">
         <is>
           <t>Dilution_field</t>
         </is>
       </c>
-      <c r="X1" s="5" t="inlineStr">
+      <c r="X1" s="6" t="inlineStr">
         <is>
           <t>ROI_field</t>
         </is>
       </c>
-      <c r="Y1" s="5" t="inlineStr">
+      <c r="Y1" s="6" t="inlineStr">
         <is>
           <t>ESD_field</t>
         </is>
       </c>
-      <c r="Z1" s="5" t="inlineStr">
+      <c r="Z1" s="6" t="inlineStr">
         <is>
           <t>ESD_unit</t>
         </is>
       </c>
-      <c r="AA1" s="5" t="inlineStr">
+      <c r="AA1" s="6" t="inlineStr">
         <is>
           <t>Biovolume_field</t>
         </is>
       </c>
-      <c r="AB1" s="5" t="inlineStr">
+      <c r="AB1" s="6" t="inlineStr">
         <is>
           <t>Biovolume_unit</t>
         </is>
       </c>
-      <c r="AC1" s="5" t="inlineStr">
+      <c r="AC1" s="6" t="inlineStr">
         <is>
           <t>Area_field</t>
         </is>
       </c>
-      <c r="AD1" s="5" t="inlineStr">
+      <c r="AD1" s="6" t="inlineStr">
         <is>
           <t>Area_unit</t>
         </is>
       </c>
-      <c r="AE1" s="5" t="inlineStr">
+      <c r="AE1" s="6" t="inlineStr">
         <is>
           <t>Minor_axis_field</t>
         </is>
       </c>
-      <c r="AF1" s="5" t="inlineStr">
+      <c r="AF1" s="6" t="inlineStr">
         <is>
           <t>Minor_axis_unit</t>
         </is>
       </c>
-      <c r="AG1" s="5" t="inlineStr">
+      <c r="AG1" s="6" t="inlineStr">
         <is>
           <t>Pixel_field</t>
         </is>
       </c>
-      <c r="AH1" s="5" t="inlineStr">
+      <c r="AH1" s="6" t="inlineStr">
         <is>
           <t>Pixel_unit</t>
         </is>
       </c>
-      <c r="AI1" s="5" t="inlineStr">
+      <c r="AI1" s="6" t="inlineStr">
         <is>
           <t>Category_field</t>
         </is>
       </c>
-      <c r="AJ1" s="5" t="inlineStr">
+      <c r="AJ1" s="6" t="inlineStr">
         <is>
           <t>Annotation_field</t>
         </is>
       </c>
-      <c r="AK1" s="5" t="inlineStr">
+      <c r="AK1" s="6" t="inlineStr">
         <is>
           <t>Flag_path</t>
         </is>
       </c>
-      <c r="AL1" s="5" t="inlineStr">
+      <c r="AL1" s="6" t="inlineStr">
         <is>
           <t>NA_value</t>
         </is>
       </c>
-      <c r="AM1" s="5" t="inlineStr">
+      <c r="AM1" s="6" t="inlineStr">
         <is>
           <t>External_project</t>
         </is>
       </c>
-      <c r="AN1" s="5" t="inlineStr">
+      <c r="AN1" s="6" t="inlineStr">
         <is>
           <t>Sampling_type_field</t>
         </is>
       </c>
-      <c r="AO1" s="5" t="inlineStr">
+      <c r="AO1" s="6" t="inlineStr">
         <is>
           <t>Sampling_lower_size_field</t>
         </is>
       </c>
-      <c r="AP1" s="5" t="inlineStr">
+      <c r="AP1" s="6" t="inlineStr">
         <is>
           <t>Sampling_lower_size_unit</t>
         </is>
       </c>
-      <c r="AQ1" s="5" t="inlineStr">
+      <c r="AQ1" s="6" t="inlineStr">
         <is>
           <t>Sampling_upper_size_field</t>
         </is>
       </c>
-      <c r="AR1" s="5" t="inlineStr">
+      <c r="AR1" s="6" t="inlineStr">
         <is>
           <t>Sampling_upper_size_unit</t>
         </is>
       </c>
-      <c r="AS1" s="5" t="inlineStr">
+      <c r="AS1" s="6" t="inlineStr">
         <is>
           <t>Sampling_description</t>
         </is>
@@ -54781,236 +54805,236 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS68"/>
+  <dimension ref="A1:AS69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Project_ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Project_source</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Project_localpath</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Instrument</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Cruise_field</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>Station_field</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
         <is>
           <t>Profile_field</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="6" t="inlineStr">
         <is>
           <t>Sample_field</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="6" t="inlineStr">
         <is>
           <t>Latitude_field</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="J1" s="6" t="inlineStr">
         <is>
           <t>Latitude_unit</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="K1" s="6" t="inlineStr">
         <is>
           <t>Longitude_field</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="L1" s="6" t="inlineStr">
         <is>
           <t>Longitude_unit</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="M1" s="6" t="inlineStr">
         <is>
           <t>Depth_min_field</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="N1" s="6" t="inlineStr">
         <is>
           <t>Depth_min_unit</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="O1" s="6" t="inlineStr">
         <is>
           <t>Depth_max_field</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="P1" s="6" t="inlineStr">
         <is>
           <t>Depth_max_unit</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="Q1" s="6" t="inlineStr">
         <is>
           <t>Sampling_date_field</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="R1" s="6" t="inlineStr">
         <is>
           <t>Sampling_date_format</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="S1" s="6" t="inlineStr">
         <is>
           <t>Sampling_time_field</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="T1" s="6" t="inlineStr">
         <is>
           <t>Sampling_time_format</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="U1" s="6" t="inlineStr">
         <is>
           <t>Volume_analyzed_field</t>
         </is>
       </c>
-      <c r="V1" s="4" t="inlineStr">
+      <c r="V1" s="6" t="inlineStr">
         <is>
           <t>Volume_analyzed_unit</t>
         </is>
       </c>
-      <c r="W1" s="4" t="inlineStr">
+      <c r="W1" s="6" t="inlineStr">
         <is>
           <t>Dilution_field</t>
         </is>
       </c>
-      <c r="X1" s="4" t="inlineStr">
+      <c r="X1" s="6" t="inlineStr">
         <is>
           <t>ROI_field</t>
         </is>
       </c>
-      <c r="Y1" s="4" t="inlineStr">
+      <c r="Y1" s="6" t="inlineStr">
         <is>
           <t>ESD_field</t>
         </is>
       </c>
-      <c r="Z1" s="4" t="inlineStr">
+      <c r="Z1" s="6" t="inlineStr">
         <is>
           <t>ESD_unit</t>
         </is>
       </c>
-      <c r="AA1" s="4" t="inlineStr">
+      <c r="AA1" s="6" t="inlineStr">
         <is>
           <t>Biovolume_field</t>
         </is>
       </c>
-      <c r="AB1" s="4" t="inlineStr">
+      <c r="AB1" s="6" t="inlineStr">
         <is>
           <t>Biovolume_unit</t>
         </is>
       </c>
-      <c r="AC1" s="4" t="inlineStr">
+      <c r="AC1" s="6" t="inlineStr">
         <is>
           <t>Area_field</t>
         </is>
       </c>
-      <c r="AD1" s="4" t="inlineStr">
+      <c r="AD1" s="6" t="inlineStr">
         <is>
           <t>Area_unit</t>
         </is>
       </c>
-      <c r="AE1" s="4" t="inlineStr">
+      <c r="AE1" s="6" t="inlineStr">
         <is>
           <t>Minor_axis_field</t>
         </is>
       </c>
-      <c r="AF1" s="4" t="inlineStr">
+      <c r="AF1" s="6" t="inlineStr">
         <is>
           <t>Minor_axis_unit</t>
         </is>
       </c>
-      <c r="AG1" s="4" t="inlineStr">
+      <c r="AG1" s="6" t="inlineStr">
         <is>
           <t>Pixel_field</t>
         </is>
       </c>
-      <c r="AH1" s="4" t="inlineStr">
+      <c r="AH1" s="6" t="inlineStr">
         <is>
           <t>Pixel_unit</t>
         </is>
       </c>
-      <c r="AI1" s="4" t="inlineStr">
+      <c r="AI1" s="6" t="inlineStr">
         <is>
           <t>Category_field</t>
         </is>
       </c>
-      <c r="AJ1" s="4" t="inlineStr">
+      <c r="AJ1" s="6" t="inlineStr">
         <is>
           <t>Annotation_field</t>
         </is>
       </c>
-      <c r="AK1" s="4" t="inlineStr">
+      <c r="AK1" s="6" t="inlineStr">
         <is>
           <t>Flag_path</t>
         </is>
       </c>
-      <c r="AL1" s="4" t="inlineStr">
+      <c r="AL1" s="6" t="inlineStr">
         <is>
           <t>NA_value</t>
         </is>
       </c>
-      <c r="AM1" s="4" t="inlineStr">
+      <c r="AM1" s="6" t="inlineStr">
         <is>
           <t>External_project</t>
         </is>
       </c>
-      <c r="AN1" s="4" t="inlineStr">
+      <c r="AN1" s="6" t="inlineStr">
         <is>
           <t>Sampling_type_field</t>
         </is>
       </c>
-      <c r="AO1" s="4" t="inlineStr">
+      <c r="AO1" s="6" t="inlineStr">
         <is>
           <t>Sampling_lower_size_field</t>
         </is>
       </c>
-      <c r="AP1" s="4" t="inlineStr">
+      <c r="AP1" s="6" t="inlineStr">
         <is>
           <t>Sampling_lower_size_unit</t>
         </is>
       </c>
-      <c r="AQ1" s="4" t="inlineStr">
+      <c r="AQ1" s="6" t="inlineStr">
         <is>
           <t>Sampling_upper_size_field</t>
         </is>
       </c>
-      <c r="AR1" s="4" t="inlineStr">
+      <c r="AR1" s="6" t="inlineStr">
         <is>
           <t>Sampling_upper_size_unit</t>
         </is>
       </c>
-      <c r="AS1" s="4" t="inlineStr">
+      <c r="AS1" s="6" t="inlineStr">
         <is>
           <t>Sampling_description</t>
         </is>
@@ -66987,6 +67011,171 @@
         </is>
       </c>
       <c r="AS68" t="inlineStr">
+        <is>
+          <t>platform:rosette;serial_number:{field:acq_sn};size_calibration_exp:{field:acq_exp};size_calibration_aa:{field:acq_aa}</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>545</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/545</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/ecotaxa_ecopart_consolidation</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>UVP</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>sample_cruise</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>sample_stationid</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>sample_profileid</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>sample_id</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>object_lat</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>degree</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>object_lon</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>degree</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>object_corrected_min_depth_bin</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>meter</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>object_corrected_max_depth_bin</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>meter</t>
+        </is>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>object_time</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>%Y-%m-%d %H:%M:%S</t>
+        </is>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>object_volume_bin</t>
+        </is>
+      </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>cubic_decimeter</t>
+        </is>
+      </c>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>object_id</t>
+        </is>
+      </c>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>object_bru_area</t>
+        </is>
+      </c>
+      <c r="AD69" t="inlineStr">
+        <is>
+          <t>square_pixel</t>
+        </is>
+      </c>
+      <c r="AG69" t="inlineStr">
+        <is>
+          <t>process_pixel</t>
+        </is>
+      </c>
+      <c r="AH69" t="inlineStr">
+        <is>
+          <t>millimeter_per_pixel</t>
+        </is>
+      </c>
+      <c r="AI69" t="inlineStr">
+        <is>
+          <t>object_annotation_category</t>
+        </is>
+      </c>
+      <c r="AJ69" t="inlineStr">
+        <is>
+          <t>object_annotation_status</t>
+        </is>
+      </c>
+      <c r="AK69" t="inlineStr">
+        <is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa_ecopart_consolidation/project_545_flags.csv</t>
+        </is>
+      </c>
+      <c r="AM69" t="inlineStr">
+        <is>
+          <t>223</t>
+        </is>
+      </c>
+      <c r="AN69" t="inlineStr">
+        <is>
+          <t>acq_instrument</t>
+        </is>
+      </c>
+      <c r="AO69" t="inlineStr">
+        <is>
+          <t>acq_smbase</t>
+        </is>
+      </c>
+      <c r="AP69" t="inlineStr">
+        <is>
+          <t>pixel</t>
+        </is>
+      </c>
+      <c r="AS69" t="inlineStr">
         <is>
           <t>platform:rosette;serial_number:{field:acq_sn};size_calibration_exp:{field:acq_exp};size_calibration_aa:{field:acq_aa}</t>
         </is>

</xml_diff>

<commit_message>
Adding daynight function to gridding, keeping minor axis for UVP consolidation, displaying both particles and vignettes nbss after standardization
</commit_message>
<xml_diff>
--- a/raw/project_UVP_standardizer.xlsx
+++ b/raw/project_UVP_standardizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCCA119-9DE2-DD4B-84D9-6A0153C7BD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE4A03A-63A0-934E-A139-823B7508F31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29300" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13669" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13823" uniqueCount="690">
   <si>
     <t>Project_ID</t>
   </si>
@@ -2552,8 +2552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="AI82" sqref="AI82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2765,6 +2765,12 @@
       <c r="AD2" t="s">
         <v>64</v>
       </c>
+      <c r="AE2" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>73</v>
+      </c>
       <c r="AG2" t="s">
         <v>65</v>
       </c>
@@ -2866,6 +2872,12 @@
       <c r="AD3" t="s">
         <v>64</v>
       </c>
+      <c r="AE3" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>73</v>
+      </c>
       <c r="AG3" t="s">
         <v>76</v>
       </c>
@@ -2967,6 +2979,12 @@
       <c r="AD4" t="s">
         <v>64</v>
       </c>
+      <c r="AE4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>73</v>
+      </c>
       <c r="AG4" t="s">
         <v>65</v>
       </c>
@@ -3068,6 +3086,12 @@
       <c r="AD5" t="s">
         <v>64</v>
       </c>
+      <c r="AE5" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>73</v>
+      </c>
       <c r="AG5" t="s">
         <v>65</v>
       </c>
@@ -3169,6 +3193,12 @@
       <c r="AD6" t="s">
         <v>64</v>
       </c>
+      <c r="AE6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>73</v>
+      </c>
       <c r="AG6" t="s">
         <v>65</v>
       </c>
@@ -3270,6 +3300,12 @@
       <c r="AD7" t="s">
         <v>64</v>
       </c>
+      <c r="AE7" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>73</v>
+      </c>
       <c r="AG7" t="s">
         <v>65</v>
       </c>
@@ -3371,6 +3407,12 @@
       <c r="AD8" t="s">
         <v>64</v>
       </c>
+      <c r="AE8" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>73</v>
+      </c>
       <c r="AG8" t="s">
         <v>65</v>
       </c>
@@ -3472,6 +3514,12 @@
       <c r="AD9" t="s">
         <v>64</v>
       </c>
+      <c r="AE9" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>73</v>
+      </c>
       <c r="AG9" t="s">
         <v>65</v>
       </c>
@@ -3573,6 +3621,12 @@
       <c r="AD10" t="s">
         <v>64</v>
       </c>
+      <c r="AE10" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>73</v>
+      </c>
       <c r="AG10" t="s">
         <v>65</v>
       </c>
@@ -3674,6 +3728,12 @@
       <c r="AD11" t="s">
         <v>64</v>
       </c>
+      <c r="AE11" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>73</v>
+      </c>
       <c r="AG11" t="s">
         <v>65</v>
       </c>
@@ -3775,6 +3835,12 @@
       <c r="AD12" t="s">
         <v>64</v>
       </c>
+      <c r="AE12" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>73</v>
+      </c>
       <c r="AG12" t="s">
         <v>65</v>
       </c>
@@ -3876,6 +3942,12 @@
       <c r="AD13" t="s">
         <v>64</v>
       </c>
+      <c r="AE13" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>73</v>
+      </c>
       <c r="AG13" t="s">
         <v>65</v>
       </c>
@@ -3977,6 +4049,12 @@
       <c r="AD14" t="s">
         <v>64</v>
       </c>
+      <c r="AE14" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>73</v>
+      </c>
       <c r="AG14" t="s">
         <v>65</v>
       </c>
@@ -4078,6 +4156,12 @@
       <c r="AD15" t="s">
         <v>64</v>
       </c>
+      <c r="AE15" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>73</v>
+      </c>
       <c r="AG15" t="s">
         <v>65</v>
       </c>
@@ -4179,6 +4263,12 @@
       <c r="AD16" t="s">
         <v>64</v>
       </c>
+      <c r="AE16" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>73</v>
+      </c>
       <c r="AG16" t="s">
         <v>65</v>
       </c>
@@ -4280,6 +4370,12 @@
       <c r="AD17" t="s">
         <v>64</v>
       </c>
+      <c r="AE17" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>73</v>
+      </c>
       <c r="AG17" t="s">
         <v>65</v>
       </c>
@@ -4381,6 +4477,12 @@
       <c r="AD18" t="s">
         <v>64</v>
       </c>
+      <c r="AE18" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>73</v>
+      </c>
       <c r="AG18" t="s">
         <v>65</v>
       </c>
@@ -4482,6 +4584,12 @@
       <c r="AD19" t="s">
         <v>64</v>
       </c>
+      <c r="AE19" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>73</v>
+      </c>
       <c r="AG19" t="s">
         <v>65</v>
       </c>
@@ -4583,6 +4691,12 @@
       <c r="AD20" t="s">
         <v>64</v>
       </c>
+      <c r="AE20" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>73</v>
+      </c>
       <c r="AG20" t="s">
         <v>65</v>
       </c>
@@ -4684,6 +4798,12 @@
       <c r="AD21" t="s">
         <v>64</v>
       </c>
+      <c r="AE21" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>73</v>
+      </c>
       <c r="AG21" t="s">
         <v>65</v>
       </c>
@@ -4785,6 +4905,12 @@
       <c r="AD22" t="s">
         <v>64</v>
       </c>
+      <c r="AE22" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>73</v>
+      </c>
       <c r="AG22" t="s">
         <v>65</v>
       </c>
@@ -4886,6 +5012,12 @@
       <c r="AD23" t="s">
         <v>64</v>
       </c>
+      <c r="AE23" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>73</v>
+      </c>
       <c r="AG23" t="s">
         <v>65</v>
       </c>
@@ -4987,6 +5119,12 @@
       <c r="AD24" t="s">
         <v>64</v>
       </c>
+      <c r="AE24" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>73</v>
+      </c>
       <c r="AG24" t="s">
         <v>65</v>
       </c>
@@ -5088,6 +5226,12 @@
       <c r="AD25" t="s">
         <v>64</v>
       </c>
+      <c r="AE25" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>73</v>
+      </c>
       <c r="AG25" t="s">
         <v>65</v>
       </c>
@@ -5189,6 +5333,12 @@
       <c r="AD26" t="s">
         <v>64</v>
       </c>
+      <c r="AE26" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>73</v>
+      </c>
       <c r="AG26" t="s">
         <v>65</v>
       </c>
@@ -5290,6 +5440,12 @@
       <c r="AD27" t="s">
         <v>64</v>
       </c>
+      <c r="AE27" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>73</v>
+      </c>
       <c r="AG27" t="s">
         <v>65</v>
       </c>
@@ -5391,6 +5547,12 @@
       <c r="AD28" t="s">
         <v>64</v>
       </c>
+      <c r="AE28" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>73</v>
+      </c>
       <c r="AG28" t="s">
         <v>65</v>
       </c>
@@ -5492,6 +5654,12 @@
       <c r="AD29" t="s">
         <v>64</v>
       </c>
+      <c r="AE29" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>73</v>
+      </c>
       <c r="AG29" t="s">
         <v>65</v>
       </c>
@@ -5593,6 +5761,12 @@
       <c r="AD30" t="s">
         <v>64</v>
       </c>
+      <c r="AE30" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>73</v>
+      </c>
       <c r="AG30" t="s">
         <v>65</v>
       </c>
@@ -5694,6 +5868,12 @@
       <c r="AD31" t="s">
         <v>64</v>
       </c>
+      <c r="AE31" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>73</v>
+      </c>
       <c r="AG31" t="s">
         <v>65</v>
       </c>
@@ -5795,6 +5975,12 @@
       <c r="AD32" t="s">
         <v>64</v>
       </c>
+      <c r="AE32" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>73</v>
+      </c>
       <c r="AG32" t="s">
         <v>65</v>
       </c>
@@ -5896,6 +6082,12 @@
       <c r="AD33" t="s">
         <v>64</v>
       </c>
+      <c r="AE33" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>73</v>
+      </c>
       <c r="AG33" t="s">
         <v>65</v>
       </c>
@@ -5997,6 +6189,12 @@
       <c r="AD34" t="s">
         <v>64</v>
       </c>
+      <c r="AE34" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>73</v>
+      </c>
       <c r="AG34" t="s">
         <v>65</v>
       </c>
@@ -6098,6 +6296,12 @@
       <c r="AD35" t="s">
         <v>64</v>
       </c>
+      <c r="AE35" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>73</v>
+      </c>
       <c r="AG35" t="s">
         <v>65</v>
       </c>
@@ -6199,6 +6403,12 @@
       <c r="AD36" t="s">
         <v>64</v>
       </c>
+      <c r="AE36" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>73</v>
+      </c>
       <c r="AG36" t="s">
         <v>65</v>
       </c>
@@ -6300,6 +6510,12 @@
       <c r="AD37" t="s">
         <v>64</v>
       </c>
+      <c r="AE37" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>73</v>
+      </c>
       <c r="AG37" t="s">
         <v>65</v>
       </c>
@@ -6401,6 +6617,12 @@
       <c r="AD38" t="s">
         <v>64</v>
       </c>
+      <c r="AE38" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>73</v>
+      </c>
       <c r="AG38" t="s">
         <v>65</v>
       </c>
@@ -6502,6 +6724,12 @@
       <c r="AD39" t="s">
         <v>64</v>
       </c>
+      <c r="AE39" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>73</v>
+      </c>
       <c r="AG39" t="s">
         <v>65</v>
       </c>
@@ -6603,6 +6831,12 @@
       <c r="AD40" t="s">
         <v>64</v>
       </c>
+      <c r="AE40" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>73</v>
+      </c>
       <c r="AG40" t="s">
         <v>65</v>
       </c>
@@ -6704,6 +6938,12 @@
       <c r="AD41" t="s">
         <v>64</v>
       </c>
+      <c r="AE41" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>73</v>
+      </c>
       <c r="AG41" t="s">
         <v>65</v>
       </c>
@@ -6805,6 +7045,12 @@
       <c r="AD42" t="s">
         <v>64</v>
       </c>
+      <c r="AE42" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>73</v>
+      </c>
       <c r="AG42" t="s">
         <v>65</v>
       </c>
@@ -6906,6 +7152,12 @@
       <c r="AD43" t="s">
         <v>64</v>
       </c>
+      <c r="AE43" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>73</v>
+      </c>
       <c r="AG43" t="s">
         <v>65</v>
       </c>
@@ -7007,6 +7259,12 @@
       <c r="AD44" t="s">
         <v>64</v>
       </c>
+      <c r="AE44" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>73</v>
+      </c>
       <c r="AG44" t="s">
         <v>65</v>
       </c>
@@ -7108,6 +7366,12 @@
       <c r="AD45" t="s">
         <v>64</v>
       </c>
+      <c r="AE45" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>73</v>
+      </c>
       <c r="AG45" t="s">
         <v>65</v>
       </c>
@@ -7209,6 +7473,12 @@
       <c r="AD46" t="s">
         <v>64</v>
       </c>
+      <c r="AE46" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>73</v>
+      </c>
       <c r="AG46" t="s">
         <v>65</v>
       </c>
@@ -7310,6 +7580,12 @@
       <c r="AD47" t="s">
         <v>64</v>
       </c>
+      <c r="AE47" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>73</v>
+      </c>
       <c r="AG47" t="s">
         <v>65</v>
       </c>
@@ -7411,6 +7687,12 @@
       <c r="AD48" t="s">
         <v>64</v>
       </c>
+      <c r="AE48" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>73</v>
+      </c>
       <c r="AG48" t="s">
         <v>65</v>
       </c>
@@ -7512,6 +7794,12 @@
       <c r="AD49" t="s">
         <v>64</v>
       </c>
+      <c r="AE49" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>73</v>
+      </c>
       <c r="AG49" t="s">
         <v>65</v>
       </c>
@@ -7613,6 +7901,12 @@
       <c r="AD50" t="s">
         <v>64</v>
       </c>
+      <c r="AE50" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>73</v>
+      </c>
       <c r="AG50" t="s">
         <v>65</v>
       </c>
@@ -7714,6 +8008,12 @@
       <c r="AD51" t="s">
         <v>64</v>
       </c>
+      <c r="AE51" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>73</v>
+      </c>
       <c r="AG51" t="s">
         <v>76</v>
       </c>
@@ -7815,6 +8115,12 @@
       <c r="AD52" t="s">
         <v>64</v>
       </c>
+      <c r="AE52" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>73</v>
+      </c>
       <c r="AG52" t="s">
         <v>76</v>
       </c>
@@ -7916,6 +8222,12 @@
       <c r="AD53" t="s">
         <v>64</v>
       </c>
+      <c r="AE53" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>73</v>
+      </c>
       <c r="AG53" t="s">
         <v>65</v>
       </c>
@@ -8011,6 +8323,12 @@
       <c r="AD54" t="s">
         <v>64</v>
       </c>
+      <c r="AE54" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>73</v>
+      </c>
       <c r="AG54" t="s">
         <v>76</v>
       </c>
@@ -8112,6 +8430,12 @@
       <c r="AD55" t="s">
         <v>64</v>
       </c>
+      <c r="AE55" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>73</v>
+      </c>
       <c r="AG55" t="s">
         <v>76</v>
       </c>
@@ -8317,6 +8641,12 @@
       <c r="AD57" t="s">
         <v>64</v>
       </c>
+      <c r="AE57" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>73</v>
+      </c>
       <c r="AG57" t="s">
         <v>76</v>
       </c>
@@ -8418,6 +8748,12 @@
       <c r="AD58" t="s">
         <v>64</v>
       </c>
+      <c r="AE58" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF58" t="s">
+        <v>73</v>
+      </c>
       <c r="AG58" t="s">
         <v>65</v>
       </c>
@@ -8513,6 +8849,12 @@
       <c r="AD59" t="s">
         <v>64</v>
       </c>
+      <c r="AE59" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>73</v>
+      </c>
       <c r="AG59" t="s">
         <v>65</v>
       </c>
@@ -8608,6 +8950,12 @@
       <c r="AD60" t="s">
         <v>64</v>
       </c>
+      <c r="AE60" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF60" t="s">
+        <v>73</v>
+      </c>
       <c r="AG60" t="s">
         <v>65</v>
       </c>
@@ -8709,6 +9057,12 @@
       <c r="AD61" t="s">
         <v>64</v>
       </c>
+      <c r="AE61" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>73</v>
+      </c>
       <c r="AG61" t="s">
         <v>76</v>
       </c>
@@ -8810,6 +9164,12 @@
       <c r="AD62" t="s">
         <v>64</v>
       </c>
+      <c r="AE62" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF62" t="s">
+        <v>73</v>
+      </c>
       <c r="AG62" t="s">
         <v>65</v>
       </c>
@@ -8911,6 +9271,12 @@
       <c r="AD63" t="s">
         <v>64</v>
       </c>
+      <c r="AE63" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF63" t="s">
+        <v>73</v>
+      </c>
       <c r="AG63" t="s">
         <v>65</v>
       </c>
@@ -9012,6 +9378,12 @@
       <c r="AD64" t="s">
         <v>64</v>
       </c>
+      <c r="AE64" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF64" t="s">
+        <v>73</v>
+      </c>
       <c r="AG64" t="s">
         <v>76</v>
       </c>
@@ -9113,6 +9485,12 @@
       <c r="AD65" t="s">
         <v>64</v>
       </c>
+      <c r="AE65" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF65" t="s">
+        <v>73</v>
+      </c>
       <c r="AG65" t="s">
         <v>65</v>
       </c>
@@ -9208,6 +9586,12 @@
       <c r="AD66" t="s">
         <v>64</v>
       </c>
+      <c r="AE66" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>73</v>
+      </c>
       <c r="AG66" t="s">
         <v>65</v>
       </c>
@@ -9303,6 +9687,12 @@
       <c r="AD67" t="s">
         <v>64</v>
       </c>
+      <c r="AE67" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>73</v>
+      </c>
       <c r="AG67" t="s">
         <v>65</v>
       </c>
@@ -9398,6 +9788,12 @@
       <c r="AD68" t="s">
         <v>64</v>
       </c>
+      <c r="AE68" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF68" t="s">
+        <v>73</v>
+      </c>
       <c r="AG68" t="s">
         <v>76</v>
       </c>
@@ -9499,6 +9895,12 @@
       <c r="AD69" t="s">
         <v>64</v>
       </c>
+      <c r="AE69" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF69" t="s">
+        <v>73</v>
+      </c>
       <c r="AG69" t="s">
         <v>76</v>
       </c>
@@ -9600,6 +10002,12 @@
       <c r="AD70" t="s">
         <v>64</v>
       </c>
+      <c r="AE70" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF70" t="s">
+        <v>73</v>
+      </c>
       <c r="AG70" t="s">
         <v>76</v>
       </c>
@@ -9701,6 +10109,12 @@
       <c r="AD71" t="s">
         <v>64</v>
       </c>
+      <c r="AE71" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF71" t="s">
+        <v>73</v>
+      </c>
       <c r="AG71" t="s">
         <v>76</v>
       </c>
@@ -9802,6 +10216,12 @@
       <c r="AD72" t="s">
         <v>64</v>
       </c>
+      <c r="AE72" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF72" t="s">
+        <v>73</v>
+      </c>
       <c r="AG72" t="s">
         <v>76</v>
       </c>
@@ -9903,6 +10323,12 @@
       <c r="AD73" t="s">
         <v>64</v>
       </c>
+      <c r="AE73" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF73" t="s">
+        <v>73</v>
+      </c>
       <c r="AG73" t="s">
         <v>76</v>
       </c>
@@ -10004,6 +10430,12 @@
       <c r="AD74" t="s">
         <v>64</v>
       </c>
+      <c r="AE74" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF74" t="s">
+        <v>73</v>
+      </c>
       <c r="AG74" t="s">
         <v>76</v>
       </c>
@@ -10105,6 +10537,12 @@
       <c r="AD75" t="s">
         <v>64</v>
       </c>
+      <c r="AE75" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF75" t="s">
+        <v>73</v>
+      </c>
       <c r="AG75" t="s">
         <v>76</v>
       </c>
@@ -10206,6 +10644,12 @@
       <c r="AD76" t="s">
         <v>64</v>
       </c>
+      <c r="AE76" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF76" t="s">
+        <v>73</v>
+      </c>
       <c r="AG76" t="s">
         <v>76</v>
       </c>
@@ -10307,6 +10751,12 @@
       <c r="AD77" t="s">
         <v>64</v>
       </c>
+      <c r="AE77" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF77" t="s">
+        <v>73</v>
+      </c>
       <c r="AG77" t="s">
         <v>76</v>
       </c>
@@ -10408,6 +10858,12 @@
       <c r="AD78" t="s">
         <v>64</v>
       </c>
+      <c r="AE78" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF78" t="s">
+        <v>73</v>
+      </c>
       <c r="AG78" t="s">
         <v>76</v>
       </c>
@@ -10508,6 +10964,12 @@
       </c>
       <c r="AD79" t="s">
         <v>64</v>
+      </c>
+      <c r="AE79" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF79" t="s">
+        <v>73</v>
       </c>
       <c r="AG79" t="s">
         <v>76</v>
@@ -37730,7 +38192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AS80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="P57" workbookViewId="0">
+      <selection activeCell="AE70" sqref="AE70:AF70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
Updating gridding and bulk nbss computation to work with additional instruments
</commit_message>
<xml_diff>
--- a/raw/project_UVP_standardizer.xlsx
+++ b/raw/project_UVP_standardizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1481CC-8E54-B84D-9118-A739239FC258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC4E9BF-A63E-3941-B9A2-AFF5EAB876B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36160" yWindow="-440" windowWidth="29300" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecotaxa" sheetId="1" r:id="rId1"/>
@@ -3147,9 +3147,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI88" sqref="AI88"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12515,6 +12515,9 @@
       <c r="AL84" t="s">
         <v>73</v>
       </c>
+      <c r="AO84">
+        <v>605</v>
+      </c>
       <c r="AP84" t="s">
         <v>76</v>
       </c>
@@ -12621,6 +12624,9 @@
       </c>
       <c r="AL85" t="s">
         <v>73</v>
+      </c>
+      <c r="AO85">
+        <v>655</v>
       </c>
       <c r="AP85" t="s">
         <v>76</v>
@@ -12762,8 +12768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU400"/>
   <sheetViews>
-    <sheetView topLeftCell="B363" workbookViewId="0">
-      <selection activeCell="B374" sqref="B374"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A362" sqref="A362:XFD362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>